<commit_message>
Adicionados Use Cases 'Efetuar reserva' e 'Finalizar reserva', tanto na especificação como no diagrama. Adicionadas duas entidades ao modelo de domínio para refletir as mudanças de use cases
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0585BDFA-696B-4CF0-992F-7E1146F8C5A9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB231623-3732-4AFB-947D-1022DACDD575}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="158">
   <si>
     <t>Actor input</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Finalizar Encomenda</t>
   </si>
   <si>
-    <t>Peças retiradas do stock</t>
-  </si>
-  <si>
     <t>2. Apresenta campos de pagamento para preencher</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Alternativa 1 [Componente incompativel] (Passo 2)</t>
   </si>
   <si>
-    <t>Apagar Seleção</t>
-  </si>
-  <si>
     <t>2. Escolhe seleção a retomar</t>
   </si>
   <si>
@@ -474,7 +468,46 @@
     <t>2. Clica para reservar</t>
   </si>
   <si>
-    <t>3. Guarda reserva</t>
+    <t>3. Guarda reserva numa lista de espera</t>
+  </si>
+  <si>
+    <t>Finalizar reserva</t>
+  </si>
+  <si>
+    <t>Ter, pelo menos, uma reserva na lista de espera</t>
+  </si>
+  <si>
+    <t>Encomenda finalizada e peças retiradas do stock</t>
+  </si>
+  <si>
+    <t>Descrição:</t>
+  </si>
+  <si>
+    <t>Envia um aviso ao cliente, informando-o que já há em stock os componentes necessários para finalizar a encomenda que tinha reservado, e que se deverá dirigir ao stand para finalizar a encomenda.</t>
+  </si>
+  <si>
+    <t>Encomenda sai da lista de espera e é guardada para ser posteriormente finalizada</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>1. Informa que componentes foram repostos e já exitem em stock</t>
+  </si>
+  <si>
+    <t>2. Determina que reservas podem ser satisfeitas com estes componentes, por ordem de antiguidade</t>
+  </si>
+  <si>
+    <t>3. Envia aviso para os respetivos clientes</t>
+  </si>
+  <si>
+    <t>4. Guarda as respetivas encomendas normalmente</t>
+  </si>
+  <si>
+    <t>5. Remove reservas/encomendas guardadas da lista de espera</t>
+  </si>
+  <si>
+    <t>Apagar Configuração</t>
   </si>
 </sst>
 </file>
@@ -520,7 +553,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -841,42 +874,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -912,6 +945,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1227,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N221"/>
+  <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="B190" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1247,40 +1286,40 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -1291,59 +1330,59 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
-        <v>52</v>
+      <c r="B12" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1351,40 +1390,40 @@
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="26"/>
+      <c r="C17" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="31"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="26"/>
+      <c r="C19" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="26"/>
+      <c r="C20" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1395,21 +1434,21 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="27"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="27"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="27"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
@@ -1418,40 +1457,40 @@
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D27" s="32"/>
     </row>
     <row r="28" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="23"/>
+      <c r="C28" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="32"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="23"/>
+      <c r="C29" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="32"/>
     </row>
     <row r="30" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="23"/>
+      <c r="C30" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="32"/>
     </row>
     <row r="31" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1462,51 +1501,51 @@
       </c>
     </row>
     <row r="32" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="24"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="24"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="24"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="24"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="24"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="25"/>
       <c r="C38" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D38" s="6"/>
     </row>
@@ -1514,20 +1553,20 @@
       <c r="B39" s="25"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
-        <v>93</v>
+      <c r="B40" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="30"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
@@ -1541,40 +1580,40 @@
       <c r="B44" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="26"/>
+      <c r="C44" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="31"/>
     </row>
     <row r="45" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="26"/>
+      <c r="C45" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="31"/>
     </row>
     <row r="46" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="31"/>
     </row>
     <row r="47" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="26"/>
+      <c r="C47" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="31"/>
     </row>
     <row r="48" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1585,51 +1624,51 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="27"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D49" s="15"/>
     </row>
     <row r="50" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="27"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="5"/>
       <c r="D50" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="27"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D51" s="16"/>
     </row>
     <row r="52" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="27"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="5"/>
       <c r="D52" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="27"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="5"/>
       <c r="D53" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="27"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D55" s="10"/>
     </row>
@@ -1637,7 +1676,7 @@
       <c r="B56" s="25"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1647,17 +1686,17 @@
     </row>
     <row r="58" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="25"/>
       <c r="C59" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D59" s="6"/>
     </row>
@@ -1665,7 +1704,7 @@
       <c r="B60" s="25"/>
       <c r="C60" s="7"/>
       <c r="D60" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1673,40 +1712,40 @@
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="26"/>
+      <c r="C63" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="31"/>
     </row>
     <row r="64" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D64" s="26"/>
+      <c r="C64" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" s="31"/>
     </row>
     <row r="65" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="26"/>
+      <c r="D65" s="31"/>
     </row>
     <row r="66" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D66" s="26"/>
+      <c r="C66" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="31"/>
     </row>
     <row r="67" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -1717,44 +1756,44 @@
       </c>
     </row>
     <row r="68" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="27"/>
+      <c r="B68" s="29"/>
       <c r="C68" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D68" s="15"/>
     </row>
     <row r="69" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="27"/>
+      <c r="B69" s="29"/>
       <c r="C69" s="5"/>
       <c r="D69" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="27"/>
+      <c r="B70" s="29"/>
       <c r="C70" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D70" s="16"/>
     </row>
     <row r="71" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="27"/>
+      <c r="B71" s="29"/>
       <c r="C71" s="5"/>
       <c r="D71" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="27"/>
+      <c r="B72" s="29"/>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D73" s="10"/>
     </row>
@@ -1762,7 +1801,7 @@
       <c r="B74" s="25"/>
       <c r="C74" s="5"/>
       <c r="D74" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1780,40 +1819,40 @@
       <c r="B78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D78" s="26"/>
+      <c r="C78" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="31"/>
     </row>
     <row r="79" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D79" s="26"/>
+      <c r="C79" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D79" s="31"/>
     </row>
     <row r="80" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D80" s="26"/>
+      <c r="C80" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="31"/>
     </row>
     <row r="81" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C81" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="26"/>
+      <c r="D81" s="31"/>
     </row>
     <row r="82" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="27" t="s">
+      <c r="B82" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -1824,28 +1863,28 @@
       </c>
     </row>
     <row r="83" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="27"/>
+      <c r="B83" s="29"/>
       <c r="C83" s="5"/>
       <c r="D83" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="27"/>
+      <c r="B84" s="29"/>
       <c r="C84" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="27"/>
+      <c r="B85" s="29"/>
       <c r="C85" s="5"/>
       <c r="D85" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="27"/>
+      <c r="B86" s="29"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
     </row>
@@ -1854,40 +1893,40 @@
       <c r="B89" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C89" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D89" s="26"/>
+      <c r="C89" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D89" s="31"/>
     </row>
     <row r="90" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C90" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D90" s="26"/>
+      <c r="C90" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D90" s="31"/>
     </row>
     <row r="91" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D91" s="26"/>
+      <c r="C91" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="31"/>
     </row>
     <row r="92" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="26"/>
+      <c r="C92" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" s="31"/>
     </row>
     <row r="93" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="27" t="s">
+      <c r="B93" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -1898,44 +1937,44 @@
       </c>
     </row>
     <row r="94" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="27"/>
+      <c r="B94" s="29"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="29"/>
+      <c r="C95" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="29"/>
+      <c r="C96" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="95" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="27"/>
-      <c r="C95" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" s="6"/>
-    </row>
-    <row r="96" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="27"/>
-      <c r="C96" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="D96" s="6"/>
     </row>
     <row r="97" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="27"/>
+      <c r="B97" s="29"/>
       <c r="C97" s="5"/>
       <c r="D97" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="27"/>
+      <c r="B98" s="29"/>
       <c r="C98" s="7"/>
       <c r="D98" s="8"/>
     </row>
     <row r="99" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D99" s="10"/>
     </row>
@@ -1943,7 +1982,7 @@
       <c r="B100" s="25"/>
       <c r="C100" s="5"/>
       <c r="D100" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1956,40 +1995,40 @@
       <c r="B104" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C104" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D104" s="23"/>
+      <c r="C104" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" s="32"/>
     </row>
     <row r="105" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D105" s="23"/>
+      <c r="C105" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D105" s="32"/>
     </row>
     <row r="106" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C106" s="22" t="s">
+      <c r="C106" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D106" s="26"/>
+      <c r="D106" s="31"/>
     </row>
     <row r="107" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C107" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D107" s="26"/>
+      <c r="C107" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D107" s="31"/>
     </row>
     <row r="108" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="28" t="s">
+      <c r="B108" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C108" s="20" t="s">
@@ -2000,17 +2039,17 @@
       </c>
     </row>
     <row r="109" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="28"/>
+      <c r="B109" s="26"/>
       <c r="C109" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D109" s="6"/>
     </row>
     <row r="110" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="28"/>
+      <c r="B110" s="26"/>
       <c r="C110" s="5"/>
       <c r="D110" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2023,40 +2062,40 @@
       <c r="B114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="22" t="s">
+      <c r="C114" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D114" s="23"/>
+      <c r="D114" s="32"/>
     </row>
     <row r="115" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D115" s="23"/>
+      <c r="C115" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D115" s="32"/>
     </row>
     <row r="116" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D116" s="26"/>
+      <c r="C116" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D116" s="31"/>
     </row>
     <row r="117" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="D117" s="26"/>
+      <c r="C117" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D117" s="31"/>
     </row>
     <row r="118" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="27" t="s">
+      <c r="B118" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="20" t="s">
@@ -2067,21 +2106,21 @@
       </c>
     </row>
     <row r="119" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="27"/>
+      <c r="B119" s="29"/>
       <c r="C119" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D119" s="6"/>
     </row>
     <row r="120" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="27"/>
+      <c r="B120" s="29"/>
       <c r="C120" s="5"/>
       <c r="D120" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="27"/>
+      <c r="B121" s="29"/>
       <c r="C121" s="7"/>
       <c r="D121" s="8"/>
     </row>
@@ -2090,40 +2129,40 @@
       <c r="B124" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C124" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D124" s="26"/>
+      <c r="C124" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D124" s="31"/>
     </row>
     <row r="125" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D125" s="26"/>
+      <c r="C125" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D125" s="31"/>
     </row>
     <row r="126" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D126" s="26"/>
+      <c r="C126" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D126" s="31"/>
     </row>
     <row r="127" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="22" t="s">
+      <c r="C127" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D127" s="26"/>
+      <c r="D127" s="31"/>
     </row>
     <row r="128" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="27" t="s">
+      <c r="B128" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C128" s="20" t="s">
@@ -2134,65 +2173,65 @@
       </c>
     </row>
     <row r="129" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="27"/>
-      <c r="C129" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="D129" s="32"/>
+      <c r="B129" s="29"/>
+      <c r="C129" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D129" s="23"/>
     </row>
     <row r="130" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="27"/>
-      <c r="C130" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="D130" s="32"/>
+      <c r="B130" s="29"/>
+      <c r="C130" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D130" s="23"/>
     </row>
     <row r="131" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="27"/>
+      <c r="B131" s="29"/>
       <c r="C131" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D131" s="6"/>
     </row>
     <row r="132" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="27"/>
+      <c r="B132" s="29"/>
       <c r="C132" s="5"/>
       <c r="D132" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="133" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="27"/>
+      <c r="B133" s="29"/>
       <c r="C133" s="5"/>
       <c r="D133" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="134" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="27"/>
+      <c r="B134" s="29"/>
       <c r="C134" s="5"/>
       <c r="D134" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="27"/>
+      <c r="B135" s="29"/>
       <c r="C135" s="7"/>
       <c r="D135" s="8"/>
     </row>
     <row r="136" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C136" s="9"/>
       <c r="D136" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="137" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="25"/>
       <c r="C137" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D137" s="6"/>
     </row>
@@ -2200,7 +2239,7 @@
       <c r="B138" s="25"/>
       <c r="C138" s="7"/>
       <c r="D138" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2208,40 +2247,40 @@
       <c r="B141" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C141" s="22" t="s">
+      <c r="C141" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D141" s="26"/>
+      <c r="D141" s="31"/>
     </row>
     <row r="142" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D142" s="26"/>
+      <c r="C142" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D142" s="31"/>
     </row>
     <row r="143" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C143" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D143" s="26"/>
+      <c r="C143" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D143" s="31"/>
     </row>
     <row r="144" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C144" s="22" t="s">
+      <c r="C144" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D144" s="26"/>
+      <c r="D144" s="31"/>
     </row>
     <row r="145" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="27" t="s">
+      <c r="B145" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C145" s="20" t="s">
@@ -2252,96 +2291,96 @@
       </c>
     </row>
     <row r="146" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="27"/>
+      <c r="B146" s="29"/>
       <c r="C146" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D146" s="6"/>
     </row>
     <row r="147" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="27"/>
+      <c r="B147" s="29"/>
       <c r="C147" s="5"/>
       <c r="D147" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="27"/>
+      <c r="B148" s="29"/>
       <c r="C148" s="5"/>
       <c r="D148" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="149" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="27"/>
+      <c r="B149" s="29"/>
       <c r="C149" s="7"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="28" t="s">
-        <v>41</v>
+      <c r="B150" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="29"/>
+      <c r="B151" s="28"/>
       <c r="C151" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D151" s="6"/>
     </row>
     <row r="152" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="30"/>
+      <c r="B152" s="27"/>
       <c r="C152" s="7"/>
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="17"/>
-      <c r="C153" s="33"/>
-      <c r="D153" s="33"/>
+      <c r="C153" s="24"/>
+      <c r="D153" s="24"/>
     </row>
     <row r="154" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="155" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C155" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="D155" s="26"/>
+      <c r="C155" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D155" s="31"/>
     </row>
     <row r="156" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C156" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D156" s="26"/>
+      <c r="C156" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D156" s="31"/>
     </row>
     <row r="157" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C157" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D157" s="26"/>
+      <c r="C157" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D157" s="31"/>
     </row>
     <row r="158" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C158" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D158" s="26"/>
+      <c r="C158" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D158" s="31"/>
     </row>
     <row r="159" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="27" t="s">
+      <c r="B159" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -2352,38 +2391,38 @@
       </c>
     </row>
     <row r="160" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="27"/>
+      <c r="B160" s="29"/>
       <c r="C160" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D160" s="6"/>
     </row>
     <row r="161" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="27"/>
+      <c r="B161" s="29"/>
       <c r="C161" s="5"/>
       <c r="D161" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="162" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="27"/>
+      <c r="B162" s="29"/>
       <c r="C162" s="5"/>
       <c r="D162" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="163" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="27"/>
+      <c r="B163" s="29"/>
       <c r="C163" s="7"/>
       <c r="D163" s="8"/>
     </row>
     <row r="164" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C164" s="9"/>
       <c r="D164" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="165" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2396,40 +2435,40 @@
       <c r="B168" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C168" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="D168" s="26"/>
+      <c r="C168" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D168" s="31"/>
     </row>
     <row r="169" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B169" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C169" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D169" s="26"/>
+      <c r="C169" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D169" s="31"/>
     </row>
     <row r="170" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B170" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="D170" s="26"/>
+      <c r="C170" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D170" s="31"/>
     </row>
     <row r="171" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B171" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C171" s="22" t="s">
+      <c r="C171" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D171" s="26"/>
+      <c r="D171" s="31"/>
     </row>
     <row r="172" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="27" t="s">
+      <c r="B172" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C172" s="3" t="s">
@@ -2440,51 +2479,51 @@
       </c>
     </row>
     <row r="173" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="27"/>
+      <c r="B173" s="29"/>
       <c r="C173" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D173" s="6"/>
     </row>
     <row r="174" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="27"/>
+      <c r="B174" s="29"/>
       <c r="C174" s="5"/>
       <c r="D174" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="175" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="27"/>
+      <c r="B175" s="29"/>
       <c r="C175" s="5"/>
       <c r="D175" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="176" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="27"/>
+      <c r="B176" s="29"/>
       <c r="C176" s="7"/>
       <c r="D176" s="8"/>
     </row>
     <row r="177" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C177" s="9"/>
       <c r="D177" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B178" s="25"/>
       <c r="C178" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D178" s="6"/>
     </row>
     <row r="179" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B179" s="25"/>
       <c r="C179" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D179" s="8"/>
     </row>
@@ -2494,11 +2533,11 @@
       <c r="D180" s="18"/>
     </row>
     <row r="181" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="34"/>
-      <c r="B181" s="34"/>
-      <c r="C181" s="34"/>
-      <c r="D181" s="34"/>
-      <c r="E181" s="34"/>
+      <c r="A181" s="19"/>
+      <c r="B181" s="19"/>
+      <c r="C181" s="19"/>
+      <c r="D181" s="19"/>
+      <c r="E181" s="19"/>
     </row>
     <row r="182" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="34"/>
@@ -2506,7 +2545,7 @@
         <v>3</v>
       </c>
       <c r="C182" s="36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D182" s="37"/>
       <c r="E182" s="34"/>
@@ -2517,7 +2556,7 @@
         <v>4</v>
       </c>
       <c r="C183" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D183" s="37"/>
       <c r="E183" s="34"/>
@@ -2528,7 +2567,7 @@
         <v>5</v>
       </c>
       <c r="C184" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D184" s="37"/>
       <c r="E184" s="34"/>
@@ -2539,7 +2578,7 @@
         <v>6</v>
       </c>
       <c r="C185" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D185" s="37"/>
       <c r="E185" s="34"/>
@@ -2562,7 +2601,7 @@
       <c r="B187" s="36"/>
       <c r="C187" s="40"/>
       <c r="D187" s="41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E187" s="34"/>
     </row>
@@ -2570,7 +2609,7 @@
       <c r="A188" s="34"/>
       <c r="B188" s="36"/>
       <c r="C188" s="40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D188" s="41"/>
       <c r="E188" s="34"/>
@@ -2580,7 +2619,7 @@
       <c r="B189" s="36"/>
       <c r="C189" s="40"/>
       <c r="D189" s="41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E189" s="34"/>
     </row>
@@ -2598,248 +2637,404 @@
       <c r="D191" s="45"/>
       <c r="E191" s="34"/>
     </row>
-    <row r="192" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="193" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B193" s="2" t="s">
+    <row r="192" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="34"/>
+      <c r="B192" s="34"/>
+      <c r="C192" s="34"/>
+      <c r="D192" s="34"/>
+      <c r="E192" s="34"/>
+    </row>
+    <row r="193" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="34"/>
+      <c r="B193" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C193" s="22" t="s">
+      <c r="C193" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D193" s="37"/>
+      <c r="E193" s="34"/>
+    </row>
+    <row r="194" spans="1:5" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="34"/>
+      <c r="B194" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C194" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="D194" s="47"/>
+      <c r="E194" s="34"/>
+    </row>
+    <row r="195" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="34"/>
+      <c r="B195" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C195" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D195" s="37"/>
+      <c r="E195" s="34"/>
+    </row>
+    <row r="196" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="34"/>
+      <c r="B196" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C196" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D196" s="37"/>
+      <c r="E196" s="34"/>
+    </row>
+    <row r="197" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="34"/>
+      <c r="B197" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D197" s="37"/>
+      <c r="E197" s="34"/>
+    </row>
+    <row r="198" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="34"/>
+      <c r="B198" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C198" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D198" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E198" s="34"/>
+    </row>
+    <row r="199" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="34"/>
+      <c r="B199" s="36"/>
+      <c r="C199" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D199" s="41"/>
+      <c r="E199" s="34"/>
+    </row>
+    <row r="200" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="34"/>
+      <c r="B200" s="36"/>
+      <c r="C200" s="40"/>
+      <c r="D200" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E200" s="34"/>
+    </row>
+    <row r="201" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="34"/>
+      <c r="B201" s="36"/>
+      <c r="C201" s="40"/>
+      <c r="D201" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E201" s="34"/>
+    </row>
+    <row r="202" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="34"/>
+      <c r="B202" s="36"/>
+      <c r="C202" s="40"/>
+      <c r="D202" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="E202" s="34"/>
+    </row>
+    <row r="203" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="34"/>
+      <c r="B203" s="36"/>
+      <c r="C203" s="42"/>
+      <c r="D203" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E203" s="34"/>
+    </row>
+    <row r="204" spans="1:5" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="17"/>
+      <c r="C204" s="18"/>
+      <c r="D204" s="18"/>
+    </row>
+    <row r="205" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="206" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D193" s="26"/>
-    </row>
-    <row r="194" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="2" t="s">
+      <c r="D206" s="31"/>
+    </row>
+    <row r="207" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C194" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D194" s="26"/>
-    </row>
-    <row r="195" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="2" t="s">
+      <c r="C207" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D207" s="31"/>
+    </row>
+    <row r="208" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C195" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D195" s="26"/>
-    </row>
-    <row r="196" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="2" t="s">
+      <c r="C208" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D208" s="31"/>
+    </row>
+    <row r="209" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B209" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C196" s="22" t="s">
+      <c r="C209" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D209" s="31"/>
+    </row>
+    <row r="210" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B210" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B211" s="29"/>
+      <c r="C211" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D211" s="6"/>
+    </row>
+    <row r="212" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="29"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D196" s="26"/>
-    </row>
-    <row r="197" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="27"/>
-      <c r="C198" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D198" s="6"/>
-    </row>
-    <row r="199" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="27"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="6" t="s">
+    </row>
+    <row r="213" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B213" s="29"/>
+      <c r="C213" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="200" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="27"/>
-      <c r="C200" s="5" t="s">
+      <c r="D213" s="6"/>
+    </row>
+    <row r="214" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B214" s="29"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D200" s="6"/>
-    </row>
-    <row r="201" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="27"/>
-      <c r="C201" s="5"/>
-      <c r="D201" s="6" t="s">
+    </row>
+    <row r="215" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B215" s="29"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="202" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="27"/>
-      <c r="C202" s="5"/>
-      <c r="D202" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="203" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="27"/>
-      <c r="C203" s="5"/>
-      <c r="D203" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="27"/>
-      <c r="C204" s="7"/>
-      <c r="D204" s="8"/>
-    </row>
-    <row r="205" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B205" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C205" s="9"/>
-      <c r="D205" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="206" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="25"/>
-      <c r="C206" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D206" s="6"/>
-    </row>
-    <row r="207" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="25"/>
-      <c r="C207" s="7"/>
-      <c r="D207" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="209" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="210" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C210" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D210" s="26"/>
-    </row>
-    <row r="211" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B211" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C211" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D211" s="26"/>
-    </row>
-    <row r="212" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B212" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C212" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D212" s="26"/>
-    </row>
-    <row r="213" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B213" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C213" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D213" s="26"/>
-    </row>
-    <row r="214" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B214" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D214" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B215" s="27"/>
-      <c r="C215" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D215" s="6"/>
-      <c r="N215" s="13"/>
-    </row>
-    <row r="216" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B216" s="27"/>
+    <row r="216" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B216" s="29"/>
       <c r="C216" s="5"/>
       <c r="D216" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B217" s="29"/>
+      <c r="C217" s="7"/>
+      <c r="D217" s="8"/>
+    </row>
+    <row r="218" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B218" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C218" s="9"/>
+      <c r="D218" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B219" s="25"/>
+      <c r="C219" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D219" s="6"/>
+    </row>
+    <row r="220" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B220" s="25"/>
+      <c r="C220" s="7"/>
+      <c r="D220" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B223" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C223" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D223" s="31"/>
+    </row>
+    <row r="224" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B224" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C224" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D224" s="31"/>
+    </row>
+    <row r="225" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B225" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C225" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D225" s="31"/>
+    </row>
+    <row r="226" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B226" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D226" s="31"/>
+    </row>
+    <row r="227" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B227" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B228" s="29"/>
+      <c r="C228" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D228" s="6"/>
+      <c r="N228" s="13"/>
+    </row>
+    <row r="229" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B229" s="29"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="230" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B230" s="29"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="231" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B231" s="29"/>
+      <c r="C231" s="7"/>
+      <c r="D231" s="8"/>
+    </row>
+    <row r="232" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B232" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C232" s="9"/>
+      <c r="D232" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="233" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B233" s="25"/>
+      <c r="C233" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D233" s="6"/>
+    </row>
+    <row r="234" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B234" s="25"/>
+      <c r="C234" s="7"/>
+      <c r="D234" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="217" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B217" s="27"/>
-      <c r="C217" s="5"/>
-      <c r="D217" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="218" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="27"/>
-      <c r="C218" s="7"/>
-      <c r="D218" s="8"/>
-    </row>
-    <row r="219" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B219" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C219" s="9"/>
-      <c r="D219" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="220" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B220" s="25"/>
-      <c r="C220" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D220" s="6"/>
-    </row>
-    <row r="221" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B221" s="25"/>
-      <c r="C221" s="7"/>
-      <c r="D221" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="93">
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C196:D196"/>
-    <mergeCell ref="B145:B149"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:B135"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="C141:D141"/>
+  <mergeCells count="99">
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="C182:D182"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="B227:B231"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="B159:B163"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C104:D104"/>
     <mergeCell ref="C183:D183"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="B93:B98"/>
+    <mergeCell ref="B232:B234"/>
+    <mergeCell ref="B150:B152"/>
     <mergeCell ref="C184:D184"/>
     <mergeCell ref="C185:D185"/>
     <mergeCell ref="B186:B190"/>
+    <mergeCell ref="C194:D194"/>
+    <mergeCell ref="B172:B176"/>
+    <mergeCell ref="B177:B179"/>
+    <mergeCell ref="C206:D206"/>
+    <mergeCell ref="C207:D207"/>
+    <mergeCell ref="C208:D208"/>
+    <mergeCell ref="C223:D223"/>
+    <mergeCell ref="C224:D224"/>
+    <mergeCell ref="C225:D225"/>
+    <mergeCell ref="C226:D226"/>
+    <mergeCell ref="B210:B217"/>
+    <mergeCell ref="B218:B220"/>
     <mergeCell ref="C156:D156"/>
     <mergeCell ref="C157:D157"/>
     <mergeCell ref="C158:D158"/>
@@ -2856,59 +3051,34 @@
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="C209:D209"/>
+    <mergeCell ref="B145:B149"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:B135"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C193:D193"/>
+    <mergeCell ref="C195:D195"/>
+    <mergeCell ref="C196:D196"/>
+    <mergeCell ref="C197:D197"/>
+    <mergeCell ref="B198:B203"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B48:B54"/>
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C210:D210"/>
-    <mergeCell ref="C211:D211"/>
-    <mergeCell ref="C212:D212"/>
-    <mergeCell ref="C213:D213"/>
-    <mergeCell ref="B197:B204"/>
-    <mergeCell ref="B205:B207"/>
-    <mergeCell ref="B172:B176"/>
-    <mergeCell ref="B177:B179"/>
-    <mergeCell ref="C193:D193"/>
-    <mergeCell ref="C194:D194"/>
-    <mergeCell ref="C195:D195"/>
     <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="B93:B98"/>
-    <mergeCell ref="B219:B221"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="B214:B218"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="B159:B163"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C155:D155"/>
     <mergeCell ref="B73:B75"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:B72"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correçao especificaçao use cases
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0585BDFA-696B-4CF0-992F-7E1146F8C5A9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6982A08-478C-4414-9E0D-C67BF0123EB0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
   <si>
     <t>Actor input</t>
   </si>
@@ -456,25 +456,7 @@
     <t>2.1. Avisa que não existe stock e pergunta se pretende guardar e/ou reservar</t>
   </si>
   <si>
-    <t>2.3. &lt;&lt;extend&gt;&gt; Efetuar Reserva</t>
-  </si>
-  <si>
     <t>2.2. &lt;&lt;extend&gt;&gt; Guardar Configuração</t>
-  </si>
-  <si>
-    <t>Efetuar reserva</t>
-  </si>
-  <si>
-    <t>Configuração reservada</t>
-  </si>
-  <si>
-    <t>1. Apresenta opção para reservar</t>
-  </si>
-  <si>
-    <t>2. Clica para reservar</t>
-  </si>
-  <si>
-    <t>3. Guarda reserva</t>
   </si>
 </sst>
 </file>
@@ -505,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,12 +497,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -841,77 +817,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1227,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N221"/>
+  <dimension ref="B1:N210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1247,40 +1187,40 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -1291,40 +1231,40 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="9"/>
@@ -1333,14 +1273,14 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>54</v>
@@ -1351,40 +1291,40 @@
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="31"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1395,21 +1335,21 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="27"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="27"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="27"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
@@ -1418,40 +1358,40 @@
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D27" s="32"/>
     </row>
     <row r="28" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="23"/>
+      <c r="D28" s="32"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="23"/>
+      <c r="D29" s="32"/>
     </row>
     <row r="30" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="32"/>
     </row>
     <row r="31" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1462,35 +1402,35 @@
       </c>
     </row>
     <row r="32" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="24"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="5" t="s">
         <v>91</v>
       </c>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="24"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="24"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="24"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="24"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
     </row>
@@ -1518,7 +1458,7 @@
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="26" t="s">
         <v>93</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -1527,7 +1467,7 @@
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="30"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
@@ -1541,40 +1481,40 @@
       <c r="B44" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="26"/>
+      <c r="D44" s="31"/>
     </row>
     <row r="45" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="26"/>
+      <c r="D45" s="31"/>
     </row>
     <row r="46" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="31"/>
     </row>
     <row r="47" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="31"/>
     </row>
     <row r="48" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1585,42 +1525,42 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="27"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="14" t="s">
         <v>70</v>
       </c>
       <c r="D49" s="15"/>
     </row>
     <row r="50" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="27"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="5"/>
       <c r="D50" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="27"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D51" s="16"/>
     </row>
     <row r="52" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="27"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="5"/>
       <c r="D52" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="27"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="5"/>
       <c r="D53" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="27"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
     </row>
@@ -1673,40 +1613,40 @@
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="31"/>
     </row>
     <row r="64" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="26"/>
+      <c r="D64" s="31"/>
     </row>
     <row r="65" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="26"/>
+      <c r="D65" s="31"/>
     </row>
     <row r="66" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D66" s="26"/>
+      <c r="D66" s="31"/>
     </row>
     <row r="67" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -1717,35 +1657,35 @@
       </c>
     </row>
     <row r="68" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="27"/>
+      <c r="B68" s="29"/>
       <c r="C68" s="14" t="s">
         <v>84</v>
       </c>
       <c r="D68" s="15"/>
     </row>
     <row r="69" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="27"/>
+      <c r="B69" s="29"/>
       <c r="C69" s="5"/>
       <c r="D69" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="27"/>
+      <c r="B70" s="29"/>
       <c r="C70" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D70" s="16"/>
     </row>
     <row r="71" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="27"/>
+      <c r="B71" s="29"/>
       <c r="C71" s="5"/>
       <c r="D71" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="27"/>
+      <c r="B72" s="29"/>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
     </row>
@@ -1780,40 +1720,40 @@
       <c r="B78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="22" t="s">
+      <c r="C78" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D78" s="26"/>
+      <c r="D78" s="31"/>
     </row>
     <row r="79" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C79" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D79" s="26"/>
+      <c r="D79" s="31"/>
     </row>
     <row r="80" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C80" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D80" s="26"/>
+      <c r="D80" s="31"/>
     </row>
     <row r="81" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C81" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="26"/>
+      <c r="D81" s="31"/>
     </row>
     <row r="82" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="27" t="s">
+      <c r="B82" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -1824,28 +1764,28 @@
       </c>
     </row>
     <row r="83" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="27"/>
+      <c r="B83" s="29"/>
       <c r="C83" s="5"/>
       <c r="D83" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="27"/>
+      <c r="B84" s="29"/>
       <c r="C84" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="27"/>
+      <c r="B85" s="29"/>
       <c r="C85" s="5"/>
       <c r="D85" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="86" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="27"/>
+      <c r="B86" s="29"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
     </row>
@@ -1854,40 +1794,40 @@
       <c r="B89" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C89" s="22" t="s">
+      <c r="C89" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D89" s="26"/>
+      <c r="D89" s="31"/>
     </row>
     <row r="90" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C90" s="22" t="s">
+      <c r="C90" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D90" s="26"/>
+      <c r="D90" s="31"/>
     </row>
     <row r="91" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="22" t="s">
+      <c r="C91" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D91" s="26"/>
+      <c r="D91" s="31"/>
     </row>
     <row r="92" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="22" t="s">
+      <c r="C92" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D92" s="26"/>
+      <c r="D92" s="31"/>
     </row>
     <row r="93" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="27" t="s">
+      <c r="B93" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -1898,35 +1838,35 @@
       </c>
     </row>
     <row r="94" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="27"/>
+      <c r="B94" s="29"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="27"/>
+      <c r="B95" s="29"/>
       <c r="C95" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D95" s="6"/>
     </row>
     <row r="96" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="27"/>
+      <c r="B96" s="29"/>
       <c r="C96" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D96" s="6"/>
     </row>
     <row r="97" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="27"/>
+      <c r="B97" s="29"/>
       <c r="C97" s="5"/>
       <c r="D97" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="27"/>
+      <c r="B98" s="29"/>
       <c r="C98" s="7"/>
       <c r="D98" s="8"/>
     </row>
@@ -1956,40 +1896,40 @@
       <c r="B104" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C104" s="22" t="s">
+      <c r="C104" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D104" s="23"/>
+      <c r="D104" s="32"/>
     </row>
     <row r="105" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="22" t="s">
+      <c r="C105" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D105" s="23"/>
+      <c r="D105" s="32"/>
     </row>
     <row r="106" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C106" s="22" t="s">
+      <c r="C106" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D106" s="26"/>
+      <c r="D106" s="31"/>
     </row>
     <row r="107" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C107" s="22" t="s">
+      <c r="C107" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="D107" s="26"/>
+      <c r="D107" s="31"/>
     </row>
     <row r="108" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="28" t="s">
+      <c r="B108" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C108" s="20" t="s">
@@ -2000,14 +1940,14 @@
       </c>
     </row>
     <row r="109" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="28"/>
+      <c r="B109" s="26"/>
       <c r="C109" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D109" s="6"/>
     </row>
     <row r="110" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="28"/>
+      <c r="B110" s="26"/>
       <c r="C110" s="5"/>
       <c r="D110" s="6" t="s">
         <v>108</v>
@@ -2023,40 +1963,40 @@
       <c r="B114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="22" t="s">
+      <c r="C114" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D114" s="23"/>
+      <c r="D114" s="32"/>
     </row>
     <row r="115" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="22" t="s">
+      <c r="C115" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D115" s="23"/>
+      <c r="D115" s="32"/>
     </row>
     <row r="116" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="22" t="s">
+      <c r="C116" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D116" s="26"/>
+      <c r="D116" s="31"/>
     </row>
     <row r="117" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="22" t="s">
+      <c r="C117" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D117" s="26"/>
+      <c r="D117" s="31"/>
     </row>
     <row r="118" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="27" t="s">
+      <c r="B118" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="20" t="s">
@@ -2067,21 +2007,21 @@
       </c>
     </row>
     <row r="119" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="27"/>
+      <c r="B119" s="29"/>
       <c r="C119" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D119" s="6"/>
     </row>
     <row r="120" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="27"/>
+      <c r="B120" s="29"/>
       <c r="C120" s="5"/>
       <c r="D120" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="27"/>
+      <c r="B121" s="29"/>
       <c r="C121" s="7"/>
       <c r="D121" s="8"/>
     </row>
@@ -2090,40 +2030,40 @@
       <c r="B124" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C124" s="22" t="s">
+      <c r="C124" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D124" s="26"/>
+      <c r="D124" s="31"/>
     </row>
     <row r="125" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="22" t="s">
+      <c r="C125" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D125" s="26"/>
+      <c r="D125" s="31"/>
     </row>
     <row r="126" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="22" t="s">
+      <c r="C126" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="D126" s="26"/>
+      <c r="D126" s="31"/>
     </row>
     <row r="127" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="22" t="s">
+      <c r="C127" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D127" s="26"/>
+      <c r="D127" s="31"/>
     </row>
     <row r="128" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="27" t="s">
+      <c r="B128" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C128" s="20" t="s">
@@ -2134,49 +2074,49 @@
       </c>
     </row>
     <row r="129" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="27"/>
-      <c r="C129" s="31" t="s">
+      <c r="B129" s="29"/>
+      <c r="C129" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D129" s="32"/>
+      <c r="D129" s="23"/>
     </row>
     <row r="130" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="27"/>
-      <c r="C130" s="31" t="s">
+      <c r="B130" s="29"/>
+      <c r="C130" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D130" s="32"/>
+      <c r="D130" s="23"/>
     </row>
     <row r="131" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="27"/>
+      <c r="B131" s="29"/>
       <c r="C131" s="5" t="s">
         <v>121</v>
       </c>
       <c r="D131" s="6"/>
     </row>
     <row r="132" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="27"/>
+      <c r="B132" s="29"/>
       <c r="C132" s="5"/>
       <c r="D132" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="133" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="27"/>
+      <c r="B133" s="29"/>
       <c r="C133" s="5"/>
       <c r="D133" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="134" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="27"/>
+      <c r="B134" s="29"/>
       <c r="C134" s="5"/>
       <c r="D134" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="135" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="27"/>
+      <c r="B135" s="29"/>
       <c r="C135" s="7"/>
       <c r="D135" s="8"/>
     </row>
@@ -2208,40 +2148,40 @@
       <c r="B141" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C141" s="22" t="s">
+      <c r="C141" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D141" s="26"/>
+      <c r="D141" s="31"/>
     </row>
     <row r="142" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="22" t="s">
+      <c r="C142" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D142" s="26"/>
+      <c r="D142" s="31"/>
     </row>
     <row r="143" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C143" s="22" t="s">
+      <c r="C143" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D143" s="26"/>
+      <c r="D143" s="31"/>
     </row>
     <row r="144" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C144" s="22" t="s">
+      <c r="C144" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D144" s="26"/>
+      <c r="D144" s="31"/>
     </row>
     <row r="145" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="27" t="s">
+      <c r="B145" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C145" s="20" t="s">
@@ -2252,33 +2192,33 @@
       </c>
     </row>
     <row r="146" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="27"/>
+      <c r="B146" s="29"/>
       <c r="C146" s="5" t="s">
         <v>122</v>
       </c>
       <c r="D146" s="6"/>
     </row>
     <row r="147" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="27"/>
+      <c r="B147" s="29"/>
       <c r="C147" s="5"/>
       <c r="D147" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="148" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="27"/>
+      <c r="B148" s="29"/>
       <c r="C148" s="5"/>
       <c r="D148" s="6" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="149" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="27"/>
+      <c r="B149" s="29"/>
       <c r="C149" s="7"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="28" t="s">
+      <c r="B150" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C150" s="5"/>
@@ -2287,61 +2227,61 @@
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="29"/>
+      <c r="B151" s="28"/>
       <c r="C151" s="5" t="s">
         <v>136</v>
       </c>
       <c r="D151" s="6"/>
     </row>
     <row r="152" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="30"/>
+      <c r="B152" s="27"/>
       <c r="C152" s="7"/>
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="17"/>
-      <c r="C153" s="33"/>
-      <c r="D153" s="33"/>
+      <c r="C153" s="24"/>
+      <c r="D153" s="24"/>
     </row>
     <row r="154" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="155" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C155" s="22" t="s">
+      <c r="C155" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="D155" s="26"/>
+      <c r="D155" s="31"/>
     </row>
     <row r="156" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C156" s="22" t="s">
+      <c r="C156" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D156" s="26"/>
+      <c r="D156" s="31"/>
     </row>
     <row r="157" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C157" s="22" t="s">
+      <c r="C157" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D157" s="26"/>
+      <c r="D157" s="31"/>
     </row>
     <row r="158" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C158" s="22" t="s">
+      <c r="C158" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="D158" s="26"/>
+      <c r="D158" s="31"/>
     </row>
     <row r="159" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="27" t="s">
+      <c r="B159" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -2352,28 +2292,28 @@
       </c>
     </row>
     <row r="160" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="27"/>
+      <c r="B160" s="29"/>
       <c r="C160" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D160" s="6"/>
     </row>
     <row r="161" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="27"/>
+      <c r="B161" s="29"/>
       <c r="C161" s="5"/>
       <c r="D161" s="6" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="162" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="27"/>
+      <c r="B162" s="29"/>
       <c r="C162" s="5"/>
       <c r="D162" s="6" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="163" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="27"/>
+      <c r="B163" s="29"/>
       <c r="C163" s="7"/>
       <c r="D163" s="8"/>
     </row>
@@ -2396,40 +2336,40 @@
       <c r="B168" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C168" s="22" t="s">
+      <c r="C168" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="D168" s="26"/>
+      <c r="D168" s="31"/>
     </row>
     <row r="169" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B169" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C169" s="22" t="s">
+      <c r="C169" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D169" s="26"/>
+      <c r="D169" s="31"/>
     </row>
     <row r="170" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B170" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="22" t="s">
+      <c r="C170" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="D170" s="26"/>
+      <c r="D170" s="31"/>
     </row>
     <row r="171" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B171" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C171" s="22" t="s">
+      <c r="C171" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D171" s="26"/>
+      <c r="D171" s="31"/>
     </row>
     <row r="172" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="27" t="s">
+      <c r="B172" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C172" s="3" t="s">
@@ -2440,32 +2380,32 @@
       </c>
     </row>
     <row r="173" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="27"/>
+      <c r="B173" s="29"/>
       <c r="C173" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D173" s="6"/>
     </row>
     <row r="174" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="27"/>
+      <c r="B174" s="29"/>
       <c r="C174" s="5"/>
       <c r="D174" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="175" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="27"/>
+      <c r="B175" s="29"/>
       <c r="C175" s="5"/>
       <c r="D175" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="176" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="27"/>
+      <c r="B176" s="29"/>
       <c r="C176" s="7"/>
       <c r="D176" s="8"/>
     </row>
-    <row r="177" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="25" t="s">
         <v>55</v>
       </c>
@@ -2474,372 +2414,290 @@
         <v>139</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B178" s="25"/>
       <c r="C178" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D178" s="6"/>
     </row>
-    <row r="179" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B179" s="25"/>
-      <c r="C179" s="7" t="s">
-        <v>140</v>
-      </c>
+      <c r="C179" s="7"/>
       <c r="D179" s="8"/>
     </row>
-    <row r="180" spans="1:5" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="17"/>
       <c r="C180" s="18"/>
       <c r="D180" s="18"/>
     </row>
-    <row r="181" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="34"/>
-      <c r="B181" s="34"/>
-      <c r="C181" s="34"/>
-      <c r="D181" s="34"/>
-      <c r="E181" s="34"/>
-    </row>
-    <row r="182" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="34"/>
-      <c r="B182" s="35" t="s">
+    <row r="181" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="182" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C182" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D182" s="37"/>
-      <c r="E182" s="34"/>
-    </row>
-    <row r="183" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="34"/>
-      <c r="B183" s="35" t="s">
+      <c r="C182" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D182" s="31"/>
+    </row>
+    <row r="183" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C183" s="36" t="s">
+      <c r="C183" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D183" s="37"/>
-      <c r="E183" s="34"/>
-    </row>
-    <row r="184" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="34"/>
-      <c r="B184" s="35" t="s">
+      <c r="D183" s="31"/>
+    </row>
+    <row r="184" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="D184" s="37"/>
-      <c r="E184" s="34"/>
-    </row>
-    <row r="185" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="34"/>
-      <c r="B185" s="35" t="s">
+      <c r="C184" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D184" s="31"/>
+    </row>
+    <row r="185" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C185" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="D185" s="37"/>
-      <c r="E185" s="34"/>
-    </row>
-    <row r="186" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="34"/>
-      <c r="B186" s="36" t="s">
+      <c r="C185" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D185" s="31"/>
+    </row>
+    <row r="186" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C186" s="38" t="s">
+      <c r="C186" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D186" s="39" t="s">
+      <c r="D186" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E186" s="34"/>
-    </row>
-    <row r="187" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="34"/>
-      <c r="B187" s="36"/>
-      <c r="C187" s="40"/>
-      <c r="D187" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="E187" s="34"/>
-    </row>
-    <row r="188" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="34"/>
-      <c r="B188" s="36"/>
-      <c r="C188" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D188" s="41"/>
-      <c r="E188" s="34"/>
-    </row>
-    <row r="189" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="34"/>
-      <c r="B189" s="36"/>
-      <c r="C189" s="40"/>
-      <c r="D189" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E189" s="34"/>
-    </row>
-    <row r="190" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="34"/>
-      <c r="B190" s="36"/>
-      <c r="C190" s="42"/>
-      <c r="D190" s="43"/>
-      <c r="E190" s="34"/>
-    </row>
-    <row r="191" spans="1:5" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="34"/>
-      <c r="B191" s="44"/>
-      <c r="C191" s="45"/>
-      <c r="D191" s="45"/>
-      <c r="E191" s="34"/>
-    </row>
-    <row r="192" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="193" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B193" s="2" t="s">
+    </row>
+    <row r="187" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="29"/>
+      <c r="C187" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D187" s="6"/>
+    </row>
+    <row r="188" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="29"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="29"/>
+      <c r="C189" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D189" s="6"/>
+    </row>
+    <row r="190" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="29"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="29"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="29"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="193" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="29"/>
+      <c r="C193" s="7"/>
+      <c r="D193" s="8"/>
+    </row>
+    <row r="194" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C194" s="9"/>
+      <c r="D194" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="195" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="25"/>
+      <c r="C195" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D195" s="6"/>
+    </row>
+    <row r="196" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="25"/>
+      <c r="C196" s="7"/>
+      <c r="D196" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="198" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="199" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C193" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D193" s="26"/>
-    </row>
-    <row r="194" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="2" t="s">
+      <c r="C199" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D199" s="31"/>
+    </row>
+    <row r="200" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C194" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D194" s="26"/>
-    </row>
-    <row r="195" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="2" t="s">
+      <c r="C200" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D200" s="31"/>
+    </row>
+    <row r="201" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C195" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D195" s="26"/>
-    </row>
-    <row r="196" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="2" t="s">
+      <c r="C201" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D201" s="31"/>
+    </row>
+    <row r="202" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B202" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C196" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D196" s="26"/>
-    </row>
-    <row r="197" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="27" t="s">
+      <c r="C202" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D202" s="31"/>
+    </row>
+    <row r="203" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B203" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C197" s="3" t="s">
+      <c r="C203" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D197" s="4" t="s">
+      <c r="D203" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="27"/>
-      <c r="C198" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D198" s="6"/>
-    </row>
-    <row r="199" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="27"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="27"/>
-      <c r="C200" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D200" s="6"/>
-    </row>
-    <row r="201" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="27"/>
-      <c r="C201" s="5"/>
-      <c r="D201" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="202" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="27"/>
-      <c r="C202" s="5"/>
-      <c r="D202" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="203" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="27"/>
-      <c r="C203" s="5"/>
-      <c r="D203" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="27"/>
-      <c r="C204" s="7"/>
-      <c r="D204" s="8"/>
-    </row>
-    <row r="205" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B205" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C205" s="9"/>
-      <c r="D205" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="206" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="25"/>
-      <c r="C206" s="5" t="s">
+    <row r="204" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="29"/>
+      <c r="C204" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D204" s="6"/>
+      <c r="N204" s="13"/>
+    </row>
+    <row r="205" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="29"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="206" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="29"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="207" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="29"/>
+      <c r="C207" s="7"/>
+      <c r="D207" s="8"/>
+    </row>
+    <row r="208" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C208" s="9"/>
+      <c r="D208" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B209" s="25"/>
+      <c r="C209" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D206" s="6"/>
-    </row>
-    <row r="207" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="25"/>
-      <c r="C207" s="7"/>
-      <c r="D207" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="209" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="210" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C210" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D210" s="26"/>
-    </row>
-    <row r="211" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B211" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C211" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D211" s="26"/>
-    </row>
-    <row r="212" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B212" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C212" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D212" s="26"/>
-    </row>
-    <row r="213" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B213" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C213" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D213" s="26"/>
-    </row>
-    <row r="214" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B214" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D214" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B215" s="27"/>
-      <c r="C215" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D215" s="6"/>
-      <c r="N215" s="13"/>
-    </row>
-    <row r="216" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B216" s="27"/>
-      <c r="C216" s="5"/>
-      <c r="D216" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="217" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B217" s="27"/>
-      <c r="C217" s="5"/>
-      <c r="D217" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="218" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="27"/>
-      <c r="C218" s="7"/>
-      <c r="D218" s="8"/>
-    </row>
-    <row r="219" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B219" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C219" s="9"/>
-      <c r="D219" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="220" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B220" s="25"/>
-      <c r="C220" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D220" s="6"/>
-    </row>
-    <row r="221" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B221" s="25"/>
-      <c r="C221" s="7"/>
-      <c r="D221" s="8" t="s">
+      <c r="D209" s="6"/>
+    </row>
+    <row r="210" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B210" s="25"/>
+      <c r="C210" s="7"/>
+      <c r="D210" s="8" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="93">
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C196:D196"/>
-    <mergeCell ref="B145:B149"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:B135"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="C141:D141"/>
+  <mergeCells count="88">
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="B203:B207"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="B159:B163"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="B93:B98"/>
+    <mergeCell ref="B208:B210"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="B172:B176"/>
+    <mergeCell ref="B177:B179"/>
     <mergeCell ref="C182:D182"/>
     <mergeCell ref="C183:D183"/>
     <mergeCell ref="C184:D184"/>
-    <mergeCell ref="C185:D185"/>
-    <mergeCell ref="B186:B190"/>
+    <mergeCell ref="C199:D199"/>
+    <mergeCell ref="C200:D200"/>
+    <mergeCell ref="C201:D201"/>
+    <mergeCell ref="C202:D202"/>
+    <mergeCell ref="B186:B193"/>
+    <mergeCell ref="B194:B196"/>
     <mergeCell ref="C156:D156"/>
     <mergeCell ref="C157:D157"/>
     <mergeCell ref="C158:D158"/>
@@ -2856,59 +2714,29 @@
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="C185:D185"/>
+    <mergeCell ref="B145:B149"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:B135"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B48:B54"/>
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C210:D210"/>
-    <mergeCell ref="C211:D211"/>
-    <mergeCell ref="C212:D212"/>
-    <mergeCell ref="C213:D213"/>
-    <mergeCell ref="B197:B204"/>
-    <mergeCell ref="B205:B207"/>
-    <mergeCell ref="B172:B176"/>
-    <mergeCell ref="B177:B179"/>
-    <mergeCell ref="C193:D193"/>
-    <mergeCell ref="C194:D194"/>
-    <mergeCell ref="C195:D195"/>
     <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="B93:B98"/>
-    <mergeCell ref="B219:B221"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="B214:B218"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="B159:B163"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C155:D155"/>
     <mergeCell ref="B73:B75"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:B72"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Use case eliminação seleção
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6982A08-478C-4414-9E0D-C67BF0123EB0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A559A4E-CF6F-4A0E-BDA0-DD5F469E042C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,9 +402,6 @@
     <t>3. Insere quantia disposta a pagar pelo cliente</t>
   </si>
   <si>
-    <t>1. Insere componente a componente</t>
-  </si>
-  <si>
     <t>2. Verifica compatibilidade componente a componente</t>
   </si>
   <si>
@@ -457,6 +454,9 @@
   </si>
   <si>
     <t>2.2. &lt;&lt;extend&gt;&gt; Guardar Configuração</t>
+  </si>
+  <si>
+    <t>1. Insere/remove componente a componente</t>
   </si>
 </sst>
 </file>
@@ -826,28 +826,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1187,40 +1187,40 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="32"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -1231,40 +1231,40 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="9"/>
@@ -1273,14 +1273,14 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
         <v>54</v>
@@ -1291,40 +1291,40 @@
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="26"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1335,21 +1335,21 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="29"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="29"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
@@ -1358,37 +1358,37 @@
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="32"/>
+      <c r="D28" s="27"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="32"/>
+      <c r="D29" s="27"/>
     </row>
     <row r="30" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="32"/>
+      <c r="D30" s="27"/>
     </row>
     <row r="31" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="33" t="s">
@@ -1435,7 +1435,7 @@
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="29" t="s">
         <v>48</v>
       </c>
       <c r="C37" s="9"/>
@@ -1444,21 +1444,21 @@
       </c>
     </row>
     <row r="38" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="25"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="25"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="30" t="s">
         <v>93</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -1467,7 +1467,7 @@
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="27"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
@@ -1481,40 +1481,40 @@
       <c r="B44" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="C44" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="31"/>
+      <c r="D44" s="26"/>
     </row>
     <row r="45" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="C45" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="31"/>
+      <c r="D45" s="26"/>
     </row>
     <row r="46" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="31"/>
+      <c r="D46" s="26"/>
     </row>
     <row r="47" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="31"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1525,47 +1525,47 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="29"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="14" t="s">
         <v>70</v>
       </c>
       <c r="D49" s="15"/>
     </row>
     <row r="50" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="29"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="5"/>
       <c r="D50" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="29"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D51" s="16"/>
     </row>
     <row r="52" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="29"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="5"/>
       <c r="D52" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="29"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="5"/>
       <c r="D53" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="29"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C55" s="9" t="s">
@@ -1574,19 +1574,19 @@
       <c r="D55" s="10"/>
     </row>
     <row r="56" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="25"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="25"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="29" t="s">
         <v>78</v>
       </c>
       <c r="C58" s="9"/>
@@ -1595,14 +1595,14 @@
       </c>
     </row>
     <row r="59" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="25"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D59" s="6"/>
     </row>
     <row r="60" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="25"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="7"/>
       <c r="D60" s="8" t="s">
         <v>81</v>
@@ -1613,40 +1613,40 @@
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="30" t="s">
+      <c r="C63" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="31"/>
+      <c r="D63" s="26"/>
     </row>
     <row r="64" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="30" t="s">
+      <c r="C64" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="31"/>
+      <c r="D64" s="26"/>
     </row>
     <row r="65" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="30" t="s">
+      <c r="C65" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="31"/>
+      <c r="D65" s="26"/>
     </row>
     <row r="66" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D66" s="31"/>
+      <c r="D66" s="26"/>
     </row>
     <row r="67" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -1657,40 +1657,40 @@
       </c>
     </row>
     <row r="68" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="29"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="14" t="s">
         <v>84</v>
       </c>
       <c r="D68" s="15"/>
     </row>
     <row r="69" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="29"/>
+      <c r="B69" s="28"/>
       <c r="C69" s="5"/>
       <c r="D69" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="29"/>
+      <c r="B70" s="28"/>
       <c r="C70" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D70" s="16"/>
     </row>
     <row r="71" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="29"/>
+      <c r="B71" s="28"/>
       <c r="C71" s="5"/>
       <c r="D71" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="29"/>
+      <c r="B72" s="28"/>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="25" t="s">
+      <c r="B73" s="29" t="s">
         <v>88</v>
       </c>
       <c r="C73" s="9" t="s">
@@ -1699,14 +1699,14 @@
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="25"/>
+      <c r="B74" s="29"/>
       <c r="C74" s="5"/>
       <c r="D74" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="25"/>
+      <c r="B75" s="29"/>
       <c r="C75" s="7"/>
       <c r="D75" s="8"/>
     </row>
@@ -1720,40 +1720,40 @@
       <c r="B78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="30" t="s">
+      <c r="C78" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="D78" s="31"/>
+      <c r="D78" s="26"/>
     </row>
     <row r="79" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="30" t="s">
+      <c r="C79" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D79" s="31"/>
+      <c r="D79" s="26"/>
     </row>
     <row r="80" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="30" t="s">
+      <c r="C80" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D80" s="31"/>
+      <c r="D80" s="26"/>
     </row>
     <row r="81" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="30" t="s">
+      <c r="C81" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="31"/>
+      <c r="D81" s="26"/>
     </row>
     <row r="82" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="29" t="s">
+      <c r="B82" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -1764,28 +1764,28 @@
       </c>
     </row>
     <row r="83" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="29"/>
+      <c r="B83" s="28"/>
       <c r="C83" s="5"/>
       <c r="D83" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="29"/>
+      <c r="B84" s="28"/>
       <c r="C84" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="29"/>
+      <c r="B85" s="28"/>
       <c r="C85" s="5"/>
       <c r="D85" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="86" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="29"/>
+      <c r="B86" s="28"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
     </row>
@@ -1794,40 +1794,40 @@
       <c r="B89" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C89" s="30" t="s">
+      <c r="C89" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D89" s="31"/>
+      <c r="D89" s="26"/>
     </row>
     <row r="90" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C90" s="30" t="s">
+      <c r="C90" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D90" s="31"/>
+      <c r="D90" s="26"/>
     </row>
     <row r="91" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="30" t="s">
+      <c r="C91" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D91" s="31"/>
+      <c r="D91" s="26"/>
     </row>
     <row r="92" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="30" t="s">
+      <c r="C92" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D92" s="31"/>
+      <c r="D92" s="26"/>
     </row>
     <row r="93" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="29" t="s">
+      <c r="B93" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -1838,40 +1838,40 @@
       </c>
     </row>
     <row r="94" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="29"/>
+      <c r="B94" s="28"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="29"/>
+      <c r="B95" s="28"/>
       <c r="C95" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D95" s="6"/>
     </row>
     <row r="96" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="29"/>
+      <c r="B96" s="28"/>
       <c r="C96" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D96" s="6"/>
     </row>
     <row r="97" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="29"/>
+      <c r="B97" s="28"/>
       <c r="C97" s="5"/>
       <c r="D97" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="29"/>
+      <c r="B98" s="28"/>
       <c r="C98" s="7"/>
       <c r="D98" s="8"/>
     </row>
     <row r="99" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="29" t="s">
         <v>107</v>
       </c>
       <c r="C99" s="9" t="s">
@@ -1880,14 +1880,14 @@
       <c r="D99" s="10"/>
     </row>
     <row r="100" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="25"/>
+      <c r="B100" s="29"/>
       <c r="C100" s="5"/>
       <c r="D100" s="6" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="101" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="25"/>
+      <c r="B101" s="29"/>
       <c r="C101" s="7"/>
       <c r="D101" s="8"/>
     </row>
@@ -1896,40 +1896,40 @@
       <c r="B104" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C104" s="30" t="s">
+      <c r="C104" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D104" s="32"/>
+      <c r="D104" s="27"/>
     </row>
     <row r="105" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="30" t="s">
+      <c r="C105" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D105" s="32"/>
+      <c r="D105" s="27"/>
     </row>
     <row r="106" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C106" s="30" t="s">
+      <c r="C106" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D106" s="31"/>
+      <c r="D106" s="26"/>
     </row>
     <row r="107" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C107" s="30" t="s">
+      <c r="C107" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D107" s="31"/>
+      <c r="D107" s="26"/>
     </row>
     <row r="108" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="26" t="s">
+      <c r="B108" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C108" s="20" t="s">
@@ -1940,21 +1940,21 @@
       </c>
     </row>
     <row r="109" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="26"/>
+      <c r="B109" s="30"/>
       <c r="C109" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D109" s="6"/>
     </row>
     <row r="110" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="26"/>
+      <c r="B110" s="30"/>
       <c r="C110" s="5"/>
       <c r="D110" s="6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="111" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="25"/>
+      <c r="B111" s="29"/>
       <c r="C111" s="7"/>
       <c r="D111" s="8"/>
     </row>
@@ -1963,40 +1963,40 @@
       <c r="B114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="30" t="s">
+      <c r="C114" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D114" s="32"/>
+      <c r="D114" s="27"/>
     </row>
     <row r="115" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="30" t="s">
+      <c r="C115" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D115" s="32"/>
+      <c r="D115" s="27"/>
     </row>
     <row r="116" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="30" t="s">
+      <c r="C116" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D116" s="31"/>
+      <c r="D116" s="26"/>
     </row>
     <row r="117" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="30" t="s">
+      <c r="C117" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D117" s="31"/>
+      <c r="D117" s="26"/>
     </row>
     <row r="118" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="29" t="s">
+      <c r="B118" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="20" t="s">
@@ -2007,21 +2007,21 @@
       </c>
     </row>
     <row r="119" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="29"/>
+      <c r="B119" s="28"/>
       <c r="C119" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D119" s="6"/>
     </row>
     <row r="120" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="29"/>
+      <c r="B120" s="28"/>
       <c r="C120" s="5"/>
       <c r="D120" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="29"/>
+      <c r="B121" s="28"/>
       <c r="C121" s="7"/>
       <c r="D121" s="8"/>
     </row>
@@ -2030,40 +2030,40 @@
       <c r="B124" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C124" s="30" t="s">
+      <c r="C124" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D124" s="31"/>
+      <c r="D124" s="26"/>
     </row>
     <row r="125" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="30" t="s">
+      <c r="C125" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D125" s="31"/>
+      <c r="D125" s="26"/>
     </row>
     <row r="126" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="D126" s="31"/>
+      <c r="C126" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D126" s="26"/>
     </row>
     <row r="127" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="30" t="s">
+      <c r="C127" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D127" s="31"/>
+      <c r="D127" s="26"/>
     </row>
     <row r="128" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="29" t="s">
+      <c r="B128" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C128" s="20" t="s">
@@ -2074,54 +2074,54 @@
       </c>
     </row>
     <row r="129" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="29"/>
+      <c r="B129" s="28"/>
       <c r="C129" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D129" s="23"/>
+    </row>
+    <row r="130" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B130" s="28"/>
+      <c r="C130" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D129" s="23"/>
-    </row>
-    <row r="130" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="29"/>
-      <c r="C130" s="22" t="s">
-        <v>133</v>
-      </c>
       <c r="D130" s="23"/>
     </row>
     <row r="131" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="29"/>
+      <c r="B131" s="28"/>
       <c r="C131" s="5" t="s">
         <v>121</v>
       </c>
       <c r="D131" s="6"/>
     </row>
     <row r="132" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="29"/>
+      <c r="B132" s="28"/>
       <c r="C132" s="5"/>
       <c r="D132" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="133" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="29"/>
+      <c r="B133" s="28"/>
       <c r="C133" s="5"/>
       <c r="D133" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="134" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="29"/>
+      <c r="B134" s="28"/>
       <c r="C134" s="5"/>
       <c r="D134" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="135" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="29"/>
+      <c r="B135" s="28"/>
       <c r="C135" s="7"/>
       <c r="D135" s="8"/>
     </row>
     <row r="136" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="25" t="s">
+      <c r="B136" s="29" t="s">
         <v>118</v>
       </c>
       <c r="C136" s="9"/>
@@ -2130,17 +2130,17 @@
       </c>
     </row>
     <row r="137" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="25"/>
+      <c r="B137" s="29"/>
       <c r="C137" s="5" t="s">
         <v>119</v>
       </c>
       <c r="D137" s="6"/>
     </row>
     <row r="138" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="25"/>
+      <c r="B138" s="29"/>
       <c r="C138" s="7"/>
       <c r="D138" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2148,40 +2148,40 @@
       <c r="B141" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C141" s="30" t="s">
+      <c r="C141" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D141" s="31"/>
+      <c r="D141" s="26"/>
     </row>
     <row r="142" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="30" t="s">
+      <c r="C142" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D142" s="31"/>
+      <c r="D142" s="26"/>
     </row>
     <row r="143" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C143" s="30" t="s">
+      <c r="C143" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D143" s="31"/>
+      <c r="D143" s="26"/>
     </row>
     <row r="144" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C144" s="30" t="s">
+      <c r="C144" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D144" s="31"/>
+      <c r="D144" s="26"/>
     </row>
     <row r="145" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="29" t="s">
+      <c r="B145" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C145" s="20" t="s">
@@ -2192,49 +2192,49 @@
       </c>
     </row>
     <row r="146" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="29"/>
+      <c r="B146" s="28"/>
       <c r="C146" s="5" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="D146" s="6"/>
     </row>
     <row r="147" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="29"/>
+      <c r="B147" s="28"/>
       <c r="C147" s="5"/>
       <c r="D147" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="148" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="29"/>
+      <c r="B148" s="28"/>
       <c r="C148" s="5"/>
       <c r="D148" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="149" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="29"/>
+      <c r="B149" s="28"/>
       <c r="C149" s="7"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="26" t="s">
+      <c r="B150" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="31"/>
+      <c r="C151" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="28"/>
-      <c r="C151" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="D151" s="6"/>
     </row>
     <row r="152" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="27"/>
+      <c r="B152" s="32"/>
       <c r="C152" s="7"/>
       <c r="D152" s="8"/>
     </row>
@@ -2248,40 +2248,40 @@
       <c r="B155" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C155" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D155" s="31"/>
+      <c r="C155" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D155" s="26"/>
     </row>
     <row r="156" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C156" s="30" t="s">
+      <c r="C156" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D156" s="31"/>
+      <c r="D156" s="26"/>
     </row>
     <row r="157" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C157" s="30" t="s">
+      <c r="C157" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D157" s="31"/>
+      <c r="D157" s="26"/>
     </row>
     <row r="158" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C158" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D158" s="31"/>
+      <c r="C158" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D158" s="26"/>
     </row>
     <row r="159" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="29" t="s">
+      <c r="B159" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -2292,42 +2292,42 @@
       </c>
     </row>
     <row r="160" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="29"/>
+      <c r="B160" s="28"/>
       <c r="C160" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D160" s="6"/>
     </row>
     <row r="161" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="29"/>
+      <c r="B161" s="28"/>
       <c r="C161" s="5"/>
       <c r="D161" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="162" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="29"/>
+      <c r="B162" s="28"/>
       <c r="C162" s="5"/>
       <c r="D162" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="163" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="29"/>
+      <c r="B163" s="28"/>
       <c r="C163" s="7"/>
       <c r="D163" s="8"/>
     </row>
     <row r="164" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="25" t="s">
-        <v>129</v>
+      <c r="B164" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="C164" s="9"/>
       <c r="D164" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="165" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="25"/>
+      <c r="B165" s="29"/>
       <c r="C165" s="7"/>
       <c r="D165" s="8"/>
     </row>
@@ -2336,40 +2336,40 @@
       <c r="B168" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C168" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="D168" s="31"/>
+      <c r="C168" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D168" s="26"/>
     </row>
     <row r="169" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B169" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C169" s="30" t="s">
+      <c r="C169" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D169" s="31"/>
+      <c r="D169" s="26"/>
     </row>
     <row r="170" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B170" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="D170" s="31"/>
+      <c r="C170" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D170" s="26"/>
     </row>
     <row r="171" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B171" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C171" s="30" t="s">
+      <c r="C171" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D171" s="31"/>
+      <c r="D171" s="26"/>
     </row>
     <row r="172" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="29" t="s">
+      <c r="B172" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C172" s="3" t="s">
@@ -2380,49 +2380,49 @@
       </c>
     </row>
     <row r="173" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="29"/>
+      <c r="B173" s="28"/>
       <c r="C173" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D173" s="6"/>
     </row>
     <row r="174" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="29"/>
+      <c r="B174" s="28"/>
       <c r="C174" s="5"/>
       <c r="D174" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="175" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="29"/>
+      <c r="B175" s="28"/>
       <c r="C175" s="5"/>
       <c r="D175" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="176" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="29"/>
+      <c r="B176" s="28"/>
       <c r="C176" s="7"/>
       <c r="D176" s="8"/>
     </row>
     <row r="177" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="25" t="s">
+      <c r="B177" s="29" t="s">
         <v>55</v>
       </c>
       <c r="C177" s="9"/>
       <c r="D177" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="29"/>
+      <c r="C178" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="178" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="25"/>
-      <c r="C178" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="D178" s="6"/>
     </row>
     <row r="179" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="25"/>
+      <c r="B179" s="29"/>
       <c r="C179" s="7"/>
       <c r="D179" s="8"/>
     </row>
@@ -2436,40 +2436,40 @@
       <c r="B182" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C182" s="30" t="s">
+      <c r="C182" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D182" s="31"/>
+      <c r="D182" s="26"/>
     </row>
     <row r="183" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B183" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C183" s="30" t="s">
+      <c r="C183" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D183" s="31"/>
+      <c r="D183" s="26"/>
     </row>
     <row r="184" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B184" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="30" t="s">
+      <c r="C184" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D184" s="31"/>
+      <c r="D184" s="26"/>
     </row>
     <row r="185" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B185" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C185" s="30" t="s">
+      <c r="C185" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D185" s="31"/>
+      <c r="D185" s="26"/>
     </row>
     <row r="186" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="29" t="s">
+      <c r="B186" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C186" s="3" t="s">
@@ -2480,54 +2480,54 @@
       </c>
     </row>
     <row r="187" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="29"/>
+      <c r="B187" s="28"/>
       <c r="C187" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D187" s="6"/>
     </row>
     <row r="188" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="29"/>
+      <c r="B188" s="28"/>
       <c r="C188" s="5"/>
       <c r="D188" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="189" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="29"/>
+      <c r="B189" s="28"/>
       <c r="C189" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D189" s="6"/>
     </row>
     <row r="190" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B190" s="29"/>
+      <c r="B190" s="28"/>
       <c r="C190" s="5"/>
       <c r="D190" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="191" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="29"/>
+      <c r="B191" s="28"/>
       <c r="C191" s="5"/>
       <c r="D191" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="192" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="29"/>
+      <c r="B192" s="28"/>
       <c r="C192" s="5"/>
       <c r="D192" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="193" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B193" s="29"/>
+      <c r="B193" s="28"/>
       <c r="C193" s="7"/>
       <c r="D193" s="8"/>
     </row>
     <row r="194" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="25" t="s">
+      <c r="B194" s="29" t="s">
         <v>46</v>
       </c>
       <c r="C194" s="9"/>
@@ -2536,14 +2536,14 @@
       </c>
     </row>
     <row r="195" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="25"/>
+      <c r="B195" s="29"/>
       <c r="C195" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D195" s="6"/>
     </row>
     <row r="196" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="25"/>
+      <c r="B196" s="29"/>
       <c r="C196" s="7"/>
       <c r="D196" s="8" t="s">
         <v>47</v>
@@ -2554,40 +2554,40 @@
       <c r="B199" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C199" s="30" t="s">
+      <c r="C199" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D199" s="31"/>
+      <c r="D199" s="26"/>
     </row>
     <row r="200" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B200" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C200" s="30" t="s">
+      <c r="C200" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D200" s="31"/>
+      <c r="D200" s="26"/>
     </row>
     <row r="201" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C201" s="30" t="s">
+      <c r="C201" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D201" s="31"/>
+      <c r="D201" s="26"/>
     </row>
     <row r="202" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C202" s="30" t="s">
+      <c r="C202" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D202" s="31"/>
+      <c r="D202" s="26"/>
     </row>
     <row r="203" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="29" t="s">
+      <c r="B203" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C203" s="3" t="s">
@@ -2598,7 +2598,7 @@
       </c>
     </row>
     <row r="204" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="29"/>
+      <c r="B204" s="28"/>
       <c r="C204" s="5" t="s">
         <v>39</v>
       </c>
@@ -2606,26 +2606,26 @@
       <c r="N204" s="13"/>
     </row>
     <row r="205" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B205" s="29"/>
+      <c r="B205" s="28"/>
       <c r="C205" s="5"/>
       <c r="D205" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="206" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="29"/>
+      <c r="B206" s="28"/>
       <c r="C206" s="5"/>
       <c r="D206" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="207" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="29"/>
+      <c r="B207" s="28"/>
       <c r="C207" s="7"/>
       <c r="D207" s="8"/>
     </row>
     <row r="208" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B208" s="25" t="s">
+      <c r="B208" s="29" t="s">
         <v>56</v>
       </c>
       <c r="C208" s="9"/>
@@ -2634,14 +2634,14 @@
       </c>
     </row>
     <row r="209" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="25"/>
+      <c r="B209" s="29"/>
       <c r="C209" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D209" s="6"/>
     </row>
     <row r="210" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="25"/>
+      <c r="B210" s="29"/>
       <c r="C210" s="7"/>
       <c r="D210" s="8" t="s">
         <v>60</v>
@@ -2649,6 +2649,83 @@
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C185:D185"/>
+    <mergeCell ref="B145:B149"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:B135"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="B93:B98"/>
+    <mergeCell ref="B208:B210"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="B172:B176"/>
+    <mergeCell ref="B177:B179"/>
+    <mergeCell ref="B186:B193"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="B203:B207"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="B159:B163"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C182:D182"/>
+    <mergeCell ref="C183:D183"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="C199:D199"/>
+    <mergeCell ref="C200:D200"/>
+    <mergeCell ref="C201:D201"/>
+    <mergeCell ref="C202:D202"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
@@ -2657,86 +2734,9 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C63:D63"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="B203:B207"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="B159:B163"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="B93:B98"/>
-    <mergeCell ref="B208:B210"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="B172:B176"/>
-    <mergeCell ref="B177:B179"/>
-    <mergeCell ref="C182:D182"/>
-    <mergeCell ref="C183:D183"/>
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="C199:D199"/>
-    <mergeCell ref="C200:D200"/>
-    <mergeCell ref="C201:D201"/>
-    <mergeCell ref="C202:D202"/>
-    <mergeCell ref="B186:B193"/>
-    <mergeCell ref="B194:B196"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C185:D185"/>
-    <mergeCell ref="B145:B149"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:B135"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="B31:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
+ diagramas de sequência - 15 ; use cases
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26230"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquefaria/Documents/3ºano/DSS/Projeto2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A559A4E-CF6F-4A0E-BDA0-DD5F469E042C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -25,9 +27,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -165,9 +164,6 @@
     <t>Apagar Seleção</t>
   </si>
   <si>
-    <t>2. Escolhe seleção a retomar</t>
-  </si>
-  <si>
     <t>3.Ativa botão finalizar encomenda</t>
   </si>
   <si>
@@ -327,9 +323,6 @@
     <t>1. Apresenta configurações</t>
   </si>
   <si>
-    <t>3.Apresenta configurações</t>
-  </si>
-  <si>
     <t>Autenticado com, pelo menos, uma configuração guardada</t>
   </si>
   <si>
@@ -360,9 +353,6 @@
     <t>Alternativa 1 [Desiste de apagar seleção] (Passo 3)</t>
   </si>
   <si>
-    <t>2. Seleciona o modelo escolhido</t>
-  </si>
-  <si>
     <t>1. Seleciona um pacote</t>
   </si>
   <si>
@@ -457,12 +447,21 @@
   </si>
   <si>
     <t>1. Insere/remove componente a componente</t>
+  </si>
+  <si>
+    <t>2. Escolhe configuração a retomar</t>
+  </si>
+  <si>
+    <t>3.Apresenta configuração</t>
+  </si>
+  <si>
+    <t>2. Confirma o modelo escolhido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -826,6 +825,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -833,24 +850,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1166,61 +1165,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="47.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="76.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="27"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="27"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="27"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -1230,101 +1229,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="30"/>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="30"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="30"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="30"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="32"/>
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
-        <v>52</v>
+    <row r="12" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="30"/>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="26"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28" t="s">
+      <c r="C20" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="32"/>
+    </row>
+    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1334,64 +1333,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="28"/>
+    <row r="22" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="26"/>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28"/>
+    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="28"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
     <row r="26" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="27"/>
-    </row>
-    <row r="28" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="33"/>
+    </row>
+    <row r="28" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="27"/>
-    </row>
-    <row r="29" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="33"/>
+    </row>
+    <row r="29" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="27"/>
-    </row>
-    <row r="30" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="33"/>
+    </row>
+    <row r="30" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="27"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="33" t="s">
+      <c r="C30" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="33"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1401,120 +1400,120 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="33"/>
+    <row r="32" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="27"/>
       <c r="C32" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="33"/>
+    <row r="33" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="27"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="33"/>
+    <row r="34" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="27"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="33"/>
+    <row r="35" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="27"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="33"/>
+    <row r="36" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="27"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="29" t="s">
-        <v>48</v>
+    <row r="37" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="25"/>
+      <c r="C38" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="29"/>
-      <c r="C38" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="29"/>
+    <row r="39" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="25"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="30" t="s">
-        <v>93</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="32"/>
+    <row r="41" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="29"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
     </row>
     <row r="43" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="26"/>
-    </row>
-    <row r="45" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="32"/>
+    </row>
+    <row r="45" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="26"/>
-    </row>
-    <row r="46" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="32"/>
+    </row>
+    <row r="46" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="26"/>
-    </row>
-    <row r="47" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="32"/>
+    </row>
+    <row r="47" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="28" t="s">
+      <c r="C47" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="32"/>
+    </row>
+    <row r="48" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1524,129 +1523,129 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="28"/>
+    <row r="49" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="26"/>
       <c r="C49" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D49" s="15"/>
     </row>
-    <row r="50" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="28"/>
+    <row r="50" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="26"/>
       <c r="C50" s="5"/>
       <c r="D50" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="28"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="26"/>
       <c r="C51" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D51" s="16"/>
     </row>
-    <row r="52" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="28"/>
+    <row r="52" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="26"/>
       <c r="C52" s="5"/>
       <c r="D52" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="28"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="26"/>
       <c r="C53" s="5"/>
       <c r="D53" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="28"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="26"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="29" t="s">
+    <row r="55" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="29"/>
+    <row r="56" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="25"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="29"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="25"/>
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="29" t="s">
-        <v>78</v>
+    <row r="58" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="25" t="s">
+        <v>77</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="25"/>
+      <c r="C59" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="29"/>
-      <c r="C59" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="29"/>
+    <row r="60" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="25"/>
       <c r="C60" s="7"/>
       <c r="D60" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="26"/>
-    </row>
-    <row r="64" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="32"/>
+    </row>
+    <row r="64" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D64" s="26"/>
-    </row>
-    <row r="65" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="32"/>
+    </row>
+    <row r="65" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="26"/>
-    </row>
-    <row r="66" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="32"/>
+    </row>
+    <row r="66" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D66" s="26"/>
-    </row>
-    <row r="67" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="28" t="s">
+      <c r="C66" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="32"/>
+    </row>
+    <row r="67" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -1656,104 +1655,104 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="28"/>
+    <row r="68" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="26"/>
       <c r="C68" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D68" s="15"/>
     </row>
-    <row r="69" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="28"/>
+    <row r="69" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="26"/>
       <c r="C69" s="5"/>
       <c r="D69" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="26"/>
+      <c r="C70" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="28"/>
-      <c r="C70" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="D70" s="16"/>
     </row>
-    <row r="71" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="28"/>
+    <row r="71" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="26"/>
       <c r="C71" s="5"/>
       <c r="D71" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="28"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="26"/>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="29" t="s">
-        <v>88</v>
+    <row r="73" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="29"/>
+    <row r="74" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="25"/>
       <c r="C74" s="5"/>
       <c r="D74" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="29"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="25"/>
       <c r="C75" s="7"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="17"/>
       <c r="C76" s="18"/>
       <c r="D76" s="18"/>
     </row>
     <row r="77" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D78" s="26"/>
-    </row>
-    <row r="79" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="32"/>
+    </row>
+    <row r="79" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D79" s="26"/>
-    </row>
-    <row r="80" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="32"/>
+    </row>
+    <row r="80" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="D80" s="26"/>
-    </row>
-    <row r="81" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="32"/>
+    </row>
+    <row r="81" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="25" t="s">
+      <c r="C81" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="26"/>
-    </row>
-    <row r="82" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="28" t="s">
+      <c r="D81" s="32"/>
+    </row>
+    <row r="82" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -1763,71 +1762,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="28"/>
+    <row r="83" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="26"/>
       <c r="C83" s="5"/>
       <c r="D83" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="28"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="26"/>
       <c r="C84" s="5" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="28"/>
+    <row r="85" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="26"/>
       <c r="C85" s="5"/>
       <c r="D85" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="28"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="26"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
     </row>
     <row r="88" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C89" s="25" t="s">
+      <c r="C89" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D89" s="26"/>
-    </row>
-    <row r="90" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D89" s="32"/>
+    </row>
+    <row r="90" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C90" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D90" s="26"/>
-    </row>
-    <row r="91" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D90" s="32"/>
+    </row>
+    <row r="91" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="D91" s="26"/>
-    </row>
-    <row r="92" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="32"/>
+    </row>
+    <row r="92" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="26"/>
-    </row>
-    <row r="93" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="28" t="s">
+      <c r="C92" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" s="32"/>
+    </row>
+    <row r="93" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -1837,99 +1836,99 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="28"/>
+    <row r="94" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="26"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="26"/>
+      <c r="C95" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="26"/>
+      <c r="C96" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="95" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="28"/>
-      <c r="C95" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" s="6"/>
-    </row>
-    <row r="96" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="28"/>
-      <c r="C96" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="28"/>
+    <row r="97" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="26"/>
       <c r="C97" s="5"/>
       <c r="D97" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="28"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="26"/>
       <c r="C98" s="7"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="29" t="s">
-        <v>107</v>
+    <row r="99" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="25" t="s">
+        <v>105</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="29"/>
+    <row r="100" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="25"/>
       <c r="C100" s="5"/>
       <c r="D100" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="29"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="25"/>
       <c r="C101" s="7"/>
       <c r="D101" s="8"/>
     </row>
     <row r="103" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C104" s="25" t="s">
+      <c r="C104" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D104" s="27"/>
-    </row>
-    <row r="105" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D104" s="33"/>
+    </row>
+    <row r="105" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D105" s="27"/>
-    </row>
-    <row r="106" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D105" s="33"/>
+    </row>
+    <row r="106" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C106" s="25" t="s">
+      <c r="C106" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D106" s="26"/>
-    </row>
-    <row r="107" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D106" s="32"/>
+    </row>
+    <row r="107" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C107" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D107" s="26"/>
-    </row>
-    <row r="108" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="30" t="s">
+      <c r="C107" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D107" s="32"/>
+    </row>
+    <row r="108" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C108" s="20" t="s">
@@ -1939,64 +1938,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="30"/>
+    <row r="109" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="28"/>
       <c r="C109" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D109" s="6"/>
     </row>
-    <row r="110" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="30"/>
+    <row r="110" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="28"/>
       <c r="C110" s="5"/>
       <c r="D110" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="29"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="25"/>
       <c r="C111" s="7"/>
       <c r="D111" s="8"/>
     </row>
     <row r="113" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="114" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="25" t="s">
+      <c r="C114" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D114" s="27"/>
-    </row>
-    <row r="115" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D114" s="33"/>
+    </row>
+    <row r="115" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D115" s="27"/>
-    </row>
-    <row r="116" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C115" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D115" s="33"/>
+    </row>
+    <row r="116" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D116" s="26"/>
-    </row>
-    <row r="117" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C116" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D116" s="32"/>
+    </row>
+    <row r="117" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D117" s="26"/>
-    </row>
-    <row r="118" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="28" t="s">
+      <c r="C117" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D117" s="32"/>
+    </row>
+    <row r="118" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="20" t="s">
@@ -2006,64 +2005,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="28"/>
+    <row r="119" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="26"/>
       <c r="C119" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D119" s="6"/>
     </row>
-    <row r="120" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="28"/>
+    <row r="120" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="26"/>
       <c r="C120" s="5"/>
       <c r="D120" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="28"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="26"/>
       <c r="C121" s="7"/>
       <c r="D121" s="8"/>
     </row>
     <row r="123" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C124" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D124" s="26"/>
-    </row>
-    <row r="125" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C124" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D124" s="32"/>
+    </row>
+    <row r="125" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D125" s="26"/>
-    </row>
-    <row r="126" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D125" s="32"/>
+    </row>
+    <row r="126" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="D126" s="26"/>
-    </row>
-    <row r="127" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D126" s="32"/>
+    </row>
+    <row r="127" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="25" t="s">
+      <c r="C127" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D127" s="26"/>
-    </row>
-    <row r="128" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="28" t="s">
+      <c r="D127" s="32"/>
+    </row>
+    <row r="128" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C128" s="20" t="s">
@@ -2073,115 +2072,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="28"/>
+    <row r="129" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="26"/>
       <c r="C129" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="23"/>
     </row>
-    <row r="130" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="28"/>
+    <row r="130" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="26"/>
       <c r="C130" s="22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="23"/>
     </row>
-    <row r="131" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="28"/>
+    <row r="131" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="26"/>
       <c r="C131" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D131" s="6"/>
     </row>
-    <row r="132" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="28"/>
+    <row r="132" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="26"/>
       <c r="C132" s="5"/>
       <c r="D132" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="133" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="28"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="26"/>
       <c r="C133" s="5"/>
       <c r="D133" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="28"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="26"/>
       <c r="C134" s="5"/>
       <c r="D134" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="135" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="28"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="26"/>
       <c r="C135" s="7"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="29" t="s">
-        <v>118</v>
+    <row r="136" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="C136" s="9"/>
       <c r="D136" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="137" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="29"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="25"/>
       <c r="C137" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D137" s="6"/>
     </row>
-    <row r="138" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="29"/>
+    <row r="138" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="25"/>
       <c r="C138" s="7"/>
       <c r="D138" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="141" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B141" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C141" s="25" t="s">
+      <c r="C141" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D141" s="26"/>
-    </row>
-    <row r="142" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D141" s="32"/>
+    </row>
+    <row r="142" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D142" s="26"/>
-    </row>
-    <row r="143" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C142" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D142" s="32"/>
+    </row>
+    <row r="143" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C143" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D143" s="26"/>
-    </row>
-    <row r="144" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C143" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D143" s="32"/>
+    </row>
+    <row r="144" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C144" s="25" t="s">
+      <c r="C144" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D144" s="26"/>
-    </row>
-    <row r="145" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="28" t="s">
+      <c r="D144" s="32"/>
+    </row>
+    <row r="145" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C145" s="20" t="s">
@@ -2191,97 +2190,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="28"/>
+    <row r="146" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="26"/>
       <c r="C146" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D146" s="6"/>
     </row>
-    <row r="147" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="28"/>
+    <row r="147" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="26"/>
       <c r="C147" s="5"/>
       <c r="D147" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="28"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="26"/>
       <c r="C148" s="5"/>
       <c r="D148" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="28"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="26"/>
       <c r="C149" s="7"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="30" t="s">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B150" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="31"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B151" s="30"/>
       <c r="C151" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D151" s="6"/>
     </row>
-    <row r="152" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="32"/>
+    <row r="152" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="29"/>
       <c r="C152" s="7"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B153" s="17"/>
       <c r="C153" s="24"/>
       <c r="D153" s="24"/>
     </row>
-    <row r="154" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="155" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B155" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C155" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="D155" s="26"/>
-    </row>
-    <row r="156" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D155" s="32"/>
+    </row>
+    <row r="156" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C156" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D156" s="26"/>
-    </row>
-    <row r="157" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D156" s="32"/>
+    </row>
+    <row r="157" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C157" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D157" s="26"/>
-    </row>
-    <row r="158" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D157" s="32"/>
+    </row>
+    <row r="158" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B158" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C158" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D158" s="26"/>
-    </row>
-    <row r="159" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="28" t="s">
+      <c r="C158" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D158" s="32"/>
+    </row>
+    <row r="159" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -2291,85 +2290,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="28"/>
+    <row r="160" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="26"/>
       <c r="C160" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D160" s="6"/>
     </row>
-    <row r="161" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="28"/>
+    <row r="161" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="26"/>
       <c r="C161" s="5"/>
       <c r="D161" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="28"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="26"/>
       <c r="C162" s="5"/>
       <c r="D162" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="28"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="26"/>
       <c r="C163" s="7"/>
       <c r="D163" s="8"/>
     </row>
-    <row r="164" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="29" t="s">
-        <v>128</v>
+    <row r="164" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="25" t="s">
+        <v>125</v>
       </c>
       <c r="C164" s="9"/>
       <c r="D164" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="29"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="25"/>
       <c r="C165" s="7"/>
       <c r="D165" s="8"/>
     </row>
-    <row r="167" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="168" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C168" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D168" s="26"/>
-    </row>
-    <row r="169" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C168" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D168" s="32"/>
+    </row>
+    <row r="169" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C169" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D169" s="26"/>
-    </row>
-    <row r="170" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D169" s="32"/>
+    </row>
+    <row r="170" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C170" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D170" s="26"/>
-    </row>
-    <row r="171" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C170" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D170" s="32"/>
+    </row>
+    <row r="171" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C171" s="25" t="s">
+      <c r="C171" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D171" s="26"/>
-    </row>
-    <row r="172" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="28" t="s">
+      <c r="D171" s="32"/>
+    </row>
+    <row r="172" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B172" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C172" s="3" t="s">
@@ -2379,97 +2378,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="28"/>
+    <row r="173" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B173" s="26"/>
       <c r="C173" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D173" s="6"/>
     </row>
-    <row r="174" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="28"/>
+    <row r="174" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="26"/>
       <c r="C174" s="5"/>
       <c r="D174" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="28"/>
+    <row r="175" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B175" s="26"/>
       <c r="C175" s="5"/>
       <c r="D175" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="28"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="26"/>
       <c r="C176" s="7"/>
       <c r="D176" s="8"/>
     </row>
-    <row r="177" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="29" t="s">
-        <v>55</v>
+    <row r="177" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="C177" s="9"/>
       <c r="D177" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="29"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="25"/>
       <c r="C178" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D178" s="6"/>
     </row>
-    <row r="179" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="29"/>
+    <row r="179" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="25"/>
       <c r="C179" s="7"/>
       <c r="D179" s="8"/>
     </row>
-    <row r="180" spans="2:4" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="17"/>
       <c r="C180" s="18"/>
       <c r="D180" s="18"/>
     </row>
-    <row r="181" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="182" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C182" s="25" t="s">
+      <c r="C182" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D182" s="26"/>
-    </row>
-    <row r="183" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D182" s="32"/>
+    </row>
+    <row r="183" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C183" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D183" s="26"/>
-    </row>
-    <row r="184" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C183" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D183" s="32"/>
+    </row>
+    <row r="184" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D184" s="26"/>
-    </row>
-    <row r="185" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C184" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D184" s="32"/>
+    </row>
+    <row r="185" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B185" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C185" s="25" t="s">
+      <c r="C185" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D185" s="26"/>
-    </row>
-    <row r="186" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="28" t="s">
+      <c r="D185" s="32"/>
+    </row>
+    <row r="186" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C186" s="3" t="s">
@@ -2479,115 +2478,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="28"/>
+    <row r="187" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="26"/>
       <c r="C187" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D187" s="6"/>
     </row>
-    <row r="188" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="28"/>
+    <row r="188" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B188" s="26"/>
       <c r="C188" s="5"/>
       <c r="D188" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="28"/>
+    <row r="189" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="26"/>
       <c r="C189" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D189" s="6"/>
     </row>
-    <row r="190" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B190" s="28"/>
+    <row r="190" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B190" s="26"/>
       <c r="C190" s="5"/>
       <c r="D190" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="191" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="28"/>
+    <row r="191" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="26"/>
       <c r="C191" s="5"/>
       <c r="D191" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="28"/>
+    <row r="192" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="26"/>
       <c r="C192" s="5"/>
       <c r="D192" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="193" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B193" s="28"/>
+    <row r="193" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B193" s="26"/>
       <c r="C193" s="7"/>
       <c r="D193" s="8"/>
     </row>
-    <row r="194" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="29" t="s">
-        <v>46</v>
+    <row r="194" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="C194" s="9"/>
       <c r="D194" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="195" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="29"/>
+    <row r="195" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="25"/>
       <c r="C195" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D195" s="6"/>
     </row>
-    <row r="196" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="29"/>
+    <row r="196" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B196" s="25"/>
       <c r="C196" s="7"/>
       <c r="D196" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="198" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="199" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="198" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C199" s="25" t="s">
+      <c r="C199" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D199" s="26"/>
-    </row>
-    <row r="200" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D199" s="32"/>
+    </row>
+    <row r="200" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B200" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C200" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D200" s="26"/>
-    </row>
-    <row r="201" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C200" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D200" s="32"/>
+    </row>
+    <row r="201" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B201" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C201" s="25" t="s">
+      <c r="C201" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D201" s="26"/>
-    </row>
-    <row r="202" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D201" s="32"/>
+    </row>
+    <row r="202" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B202" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C202" s="25" t="s">
+      <c r="C202" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D202" s="26"/>
-    </row>
-    <row r="203" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="28" t="s">
+      <c r="D202" s="32"/>
+    </row>
+    <row r="203" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B203" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C203" s="3" t="s">
@@ -2597,88 +2596,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="28"/>
+    <row r="204" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="26"/>
       <c r="C204" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D204" s="6"/>
       <c r="N204" s="13"/>
     </row>
-    <row r="205" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B205" s="28"/>
+    <row r="205" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B205" s="26"/>
       <c r="C205" s="5"/>
       <c r="D205" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="206" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="28"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="206" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="26"/>
       <c r="C206" s="5"/>
       <c r="D206" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="207" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="28"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="207" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B207" s="26"/>
       <c r="C207" s="7"/>
       <c r="D207" s="8"/>
     </row>
-    <row r="208" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B208" s="29" t="s">
-        <v>56</v>
+    <row r="208" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B208" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="C208" s="9"/>
       <c r="D208" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="29"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="25"/>
       <c r="C209" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D209" s="6"/>
     </row>
-    <row r="210" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="29"/>
+    <row r="210" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B210" s="25"/>
       <c r="C210" s="7"/>
       <c r="D210" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C185:D185"/>
-    <mergeCell ref="B145:B149"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:B135"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="B93:B98"/>
-    <mergeCell ref="B208:B210"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="B172:B176"/>
-    <mergeCell ref="B177:B179"/>
-    <mergeCell ref="B186:B193"/>
-    <mergeCell ref="B194:B196"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C201:D201"/>
+    <mergeCell ref="C202:D202"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C182:D182"/>
+    <mergeCell ref="C183:D183"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="C199:D199"/>
+    <mergeCell ref="C200:D200"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="B159:B163"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C170:D170"/>
     <mergeCell ref="C104:D104"/>
     <mergeCell ref="C168:D168"/>
     <mergeCell ref="C169:D169"/>
@@ -2692,51 +2705,37 @@
     <mergeCell ref="C117:D117"/>
     <mergeCell ref="C124:D124"/>
     <mergeCell ref="C114:D114"/>
+    <mergeCell ref="B208:B210"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="B172:B176"/>
+    <mergeCell ref="B177:B179"/>
+    <mergeCell ref="B186:B193"/>
+    <mergeCell ref="B194:B196"/>
     <mergeCell ref="B203:B207"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="B159:B163"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C182:D182"/>
-    <mergeCell ref="C183:D183"/>
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="C199:D199"/>
-    <mergeCell ref="C200:D200"/>
-    <mergeCell ref="C201:D201"/>
-    <mergeCell ref="C202:D202"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C185:D185"/>
+    <mergeCell ref="B145:B149"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:B135"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="B93:B98"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B37:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixes em tudo segundo o que o stor disse
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -1,38 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26230"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquefaria/Documents/3ºano/DSS/Projeto2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1 MEGA Sync\FW\UM\3 ano\DSS\Projeto2DSS-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66C4963A-258A-40F7-96D4-35F757DEA564}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="156">
   <si>
     <t>Actor input</t>
   </si>
@@ -356,9 +352,6 @@
     <t>1.seleciona configuração ótima</t>
   </si>
   <si>
-    <t>2.Apresenta janela de configuração ótimo</t>
-  </si>
-  <si>
     <t>3.seleciona pinturas</t>
   </si>
   <si>
@@ -368,9 +361,6 @@
     <t>5. Seleciona pintura</t>
   </si>
   <si>
-    <t>6.seleciona motores</t>
-  </si>
-  <si>
     <t>7.Apresenta motores disponíveis</t>
   </si>
   <si>
@@ -504,12 +494,15 @@
   </si>
   <si>
     <t>4.1.Avisa que os dados inseridos estão errados/inválidos</t>
+  </si>
+  <si>
+    <t>2.Apresenta janela de configuração ótima</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -873,37 +866,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1219,60 +1212,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="76.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="76.625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="26"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="26"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="35"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="26"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="26"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="35"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
@@ -1283,114 +1276,114 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="31"/>
-      <c r="C7" s="34" t="s">
+    <row r="7" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
+      <c r="C7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D7" s="35"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="31"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="31"/>
-      <c r="C9" s="5" t="s">
-        <v>151</v>
-      </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="31"/>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="31"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="31"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="31"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="31"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
       <c r="C15" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="31"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="27"/>
-    </row>
-    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="27"/>
-    </row>
-    <row r="21" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="34"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="34"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="27"/>
-    </row>
-    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="34"/>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="28" t="s">
         <v>2</v>
       </c>
@@ -1401,64 +1394,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="28"/>
       <c r="C24" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="28"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="28"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
     </row>
     <row r="28" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="26"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="26"/>
-    </row>
-    <row r="33" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="33" t="s">
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="20" t="s">
@@ -1468,133 +1461,133 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33"/>
-      <c r="C34" s="34" t="s">
+    <row r="34" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="29"/>
+      <c r="C34" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="29"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="29"/>
+      <c r="C36" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="35"/>
-    </row>
-    <row r="35" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="35" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="33"/>
-      <c r="C36" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="33"/>
+    <row r="37" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="29"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="33"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="29"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="33"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="29"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="33"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="29"/>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="29" t="s">
-        <v>148</v>
+    <row r="41" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="27" t="s">
+        <v>146</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="29"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="27"/>
       <c r="C42" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="29"/>
+    <row r="43" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="27"/>
       <c r="C43" s="7"/>
       <c r="D43" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="32"/>
+    <row r="45" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="31"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
     </row>
-    <row r="46" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="17"/>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
     </row>
     <row r="47" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="27"/>
-    </row>
-    <row r="49" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="34"/>
+    </row>
+    <row r="49" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="27"/>
-    </row>
-    <row r="50" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="34"/>
+    </row>
+    <row r="50" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="27"/>
-    </row>
-    <row r="51" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="34"/>
+    </row>
+    <row r="51" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="27"/>
-    </row>
-    <row r="52" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="34"/>
+    </row>
+    <row r="52" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="28" t="s">
         <v>2</v>
       </c>
@@ -1605,48 +1598,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="28"/>
       <c r="C53" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D53" s="15"/>
     </row>
-    <row r="54" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="28"/>
       <c r="C54" s="5"/>
       <c r="D54" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="28"/>
       <c r="C55" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D55" s="16"/>
     </row>
-    <row r="56" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="28"/>
       <c r="C56" s="5"/>
       <c r="D56" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="28"/>
       <c r="C57" s="5"/>
       <c r="D57" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="28"/>
       <c r="C58" s="7"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="29" t="s">
+    <row r="59" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="27" t="s">
         <v>50</v>
       </c>
       <c r="C59" s="9" t="s">
@@ -1654,20 +1647,20 @@
       </c>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="29"/>
+    <row r="60" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="27"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="29"/>
+    <row r="61" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="27"/>
       <c r="C61" s="7"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="29" t="s">
+    <row r="62" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="27" t="s">
         <v>56</v>
       </c>
       <c r="C62" s="9"/>
@@ -1675,58 +1668,58 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="29"/>
+    <row r="63" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="27"/>
       <c r="C63" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="29"/>
+    <row r="64" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="27"/>
       <c r="C64" s="7"/>
       <c r="D64" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="27"/>
-    </row>
-    <row r="68" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="34"/>
+    </row>
+    <row r="68" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="27"/>
-    </row>
-    <row r="69" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="34"/>
+    </row>
+    <row r="69" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="27"/>
-    </row>
-    <row r="70" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="34"/>
+    </row>
+    <row r="70" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="D70" s="27"/>
-    </row>
-    <row r="71" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="34"/>
+    </row>
+    <row r="71" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="28" t="s">
         <v>2</v>
       </c>
@@ -1737,41 +1730,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="28"/>
       <c r="C72" s="14" t="s">
         <v>62</v>
       </c>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="28"/>
       <c r="C73" s="5"/>
       <c r="D73" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="28"/>
       <c r="C74" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D74" s="16"/>
     </row>
-    <row r="75" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="28"/>
       <c r="C75" s="5"/>
       <c r="D75" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="28"/>
       <c r="C76" s="7"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="29" t="s">
+    <row r="77" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="27" t="s">
         <v>66</v>
       </c>
       <c r="C77" s="9" t="s">
@@ -1779,61 +1772,61 @@
       </c>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="29"/>
+    <row r="78" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="27"/>
       <c r="C78" s="5"/>
       <c r="D78" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="29"/>
+    <row r="79" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="27"/>
       <c r="C79" s="7"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="17"/>
       <c r="C80" s="18"/>
       <c r="D80" s="18"/>
     </row>
     <row r="81" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C82" s="25" t="s">
+      <c r="C82" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D82" s="27"/>
-    </row>
-    <row r="83" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="34"/>
+    </row>
+    <row r="83" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="25" t="s">
+      <c r="C83" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D83" s="27"/>
-    </row>
-    <row r="84" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="34"/>
+    </row>
+    <row r="84" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C84" s="25" t="s">
+      <c r="C84" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D84" s="27"/>
-    </row>
-    <row r="85" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D84" s="34"/>
+    </row>
+    <row r="85" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C85" s="25" t="s">
+      <c r="C85" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D85" s="27"/>
-    </row>
-    <row r="86" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="34"/>
+    </row>
+    <row r="86" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="28" t="s">
         <v>2</v>
       </c>
@@ -1844,77 +1837,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="28"/>
-      <c r="C87" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D87" s="35"/>
-    </row>
-    <row r="88" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D87" s="26"/>
+    </row>
+    <row r="88" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="28"/>
       <c r="C88" s="5"/>
       <c r="D88" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="28"/>
       <c r="C89" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="28"/>
       <c r="C90" s="5"/>
       <c r="D90" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="28"/>
       <c r="C91" s="7"/>
       <c r="D91" s="8"/>
     </row>
     <row r="93" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C94" s="25" t="s">
+      <c r="C94" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D94" s="27"/>
-    </row>
-    <row r="95" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D94" s="34"/>
+    </row>
+    <row r="95" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C95" s="25" t="s">
+      <c r="C95" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D95" s="27"/>
-    </row>
-    <row r="96" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="34"/>
+    </row>
+    <row r="96" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C96" s="25" t="s">
+      <c r="C96" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D96" s="27"/>
-    </row>
-    <row r="97" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="34"/>
+    </row>
+    <row r="97" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C97" s="25" t="s">
+      <c r="C97" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D97" s="27"/>
-    </row>
-    <row r="98" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="34"/>
+    </row>
+    <row r="98" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="28" t="s">
         <v>2</v>
       </c>
@@ -1925,105 +1918,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="28"/>
-      <c r="C99" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="D99" s="35"/>
-    </row>
-    <row r="100" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D99" s="26"/>
+    </row>
+    <row r="100" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="28"/>
       <c r="C100" s="5"/>
       <c r="D100" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="28"/>
       <c r="C101" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="28"/>
       <c r="C102" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D102" s="6"/>
     </row>
-    <row r="103" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="28"/>
       <c r="C103" s="5"/>
       <c r="D103" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="28"/>
       <c r="C104" s="7"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="29" t="s">
+    <row r="105" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="27" t="s">
         <v>73</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="29"/>
+    <row r="106" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="27"/>
       <c r="C106" s="5"/>
       <c r="D106" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="29"/>
+    <row r="107" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="27"/>
       <c r="C107" s="7"/>
       <c r="D107" s="8"/>
     </row>
     <row r="109" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C110" s="25" t="s">
+      <c r="C110" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D110" s="26"/>
-    </row>
-    <row r="111" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="35"/>
+    </row>
+    <row r="111" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="25" t="s">
+      <c r="C111" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D111" s="26"/>
-    </row>
-    <row r="112" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="35"/>
+    </row>
+    <row r="112" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C112" s="25" t="s">
+      <c r="C112" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D112" s="27"/>
-    </row>
-    <row r="113" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D112" s="34"/>
+    </row>
+    <row r="113" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C113" s="25" t="s">
+      <c r="C113" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D113" s="27"/>
-    </row>
-    <row r="114" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="34"/>
+    </row>
+    <row r="114" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114" s="30" t="s">
         <v>2</v>
       </c>
@@ -2034,77 +2027,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="30"/>
-      <c r="C115" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="D115" s="35"/>
-    </row>
-    <row r="116" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C115" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D115" s="26"/>
+    </row>
+    <row r="116" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="30"/>
-      <c r="C116" s="34"/>
-      <c r="D116" s="35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C116" s="25"/>
+      <c r="D116" s="26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="30"/>
       <c r="C117" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D117" s="6"/>
     </row>
-    <row r="118" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="30"/>
       <c r="C118" s="5"/>
       <c r="D118" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="29"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="27"/>
       <c r="C119" s="7"/>
       <c r="D119" s="8"/>
     </row>
     <row r="121" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C122" s="25" t="s">
+      <c r="C122" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D122" s="26"/>
-    </row>
-    <row r="123" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D122" s="35"/>
+    </row>
+    <row r="123" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="25" t="s">
+      <c r="C123" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D123" s="26"/>
-    </row>
-    <row r="124" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D123" s="35"/>
+    </row>
+    <row r="124" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C124" s="25" t="s">
+      <c r="C124" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D124" s="27"/>
-    </row>
-    <row r="125" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="34"/>
+    </row>
+    <row r="125" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C125" s="25" t="s">
+      <c r="C125" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D125" s="27"/>
-    </row>
-    <row r="126" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D125" s="34"/>
+    </row>
+    <row r="126" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="28" t="s">
         <v>2</v>
       </c>
@@ -2115,77 +2108,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="28"/>
-      <c r="C127" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="D127" s="35"/>
-    </row>
-    <row r="128" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D127" s="26"/>
+    </row>
+    <row r="128" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="28"/>
-      <c r="C128" s="34"/>
-      <c r="D128" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C128" s="25"/>
+      <c r="D128" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="28"/>
       <c r="C129" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D129" s="6"/>
     </row>
-    <row r="130" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="28"/>
       <c r="C130" s="5"/>
       <c r="D130" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="28"/>
       <c r="C131" s="7"/>
       <c r="D131" s="8"/>
     </row>
     <row r="133" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C134" s="25" t="s">
+      <c r="C134" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="D134" s="27"/>
-    </row>
-    <row r="135" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="34"/>
+    </row>
+    <row r="135" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C135" s="25" t="s">
+      <c r="C135" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D135" s="27"/>
-    </row>
-    <row r="136" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D135" s="34"/>
+    </row>
+    <row r="136" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C136" s="25" t="s">
+      <c r="C136" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="D136" s="27"/>
-    </row>
-    <row r="137" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D136" s="34"/>
+    </row>
+    <row r="137" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C137" s="25" t="s">
+      <c r="C137" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D137" s="27"/>
-    </row>
-    <row r="138" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D137" s="34"/>
+    </row>
+    <row r="138" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="28" t="s">
         <v>2</v>
       </c>
@@ -2196,156 +2189,154 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="28"/>
-      <c r="C139" s="34" t="s">
+      <c r="C139" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D139" s="35"/>
-    </row>
-    <row r="140" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="26"/>
+    </row>
+    <row r="140" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="28"/>
-      <c r="C140" s="34"/>
-      <c r="D140" s="35" t="s">
+      <c r="C140" s="25"/>
+      <c r="D140" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="28"/>
+      <c r="C141" s="25" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="141" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="28"/>
-      <c r="C141" s="34" t="s">
+      <c r="D141" s="26"/>
+    </row>
+    <row r="142" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="28"/>
+      <c r="C142" s="25"/>
+      <c r="D142" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="D141" s="35"/>
-    </row>
-    <row r="142" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="28"/>
-      <c r="C142" s="34"/>
-      <c r="D142" s="35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="143" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
       <c r="C143" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D143" s="23"/>
+    </row>
+    <row r="144" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="28"/>
+      <c r="C144" s="22"/>
+      <c r="D144" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D143" s="23"/>
-    </row>
-    <row r="144" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="28"/>
-      <c r="C144" s="22" t="s">
+    </row>
+    <row r="145" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B145" s="28"/>
+      <c r="C145" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D144" s="23"/>
-    </row>
-    <row r="145" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="28"/>
-      <c r="C145" s="22"/>
-      <c r="D145" s="23" t="s">
+      <c r="D145" s="16"/>
+    </row>
+    <row r="146" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B146" s="28"/>
+      <c r="C146" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="146" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="28"/>
-      <c r="C146" s="22" t="s">
+      <c r="D146" s="23"/>
+    </row>
+    <row r="147" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="28"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D146" s="23"/>
-    </row>
-    <row r="147" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="28"/>
-      <c r="C147" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D147" s="6"/>
-    </row>
-    <row r="148" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B148" s="28"/>
       <c r="C148" s="5"/>
       <c r="D148" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="28"/>
       <c r="C149" s="5"/>
       <c r="D149" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="150" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="28"/>
       <c r="C150" s="5"/>
-      <c r="D150" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D150" s="16"/>
+    </row>
+    <row r="151" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="28"/>
       <c r="C151" s="7"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="29" t="s">
+    <row r="152" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="27" t="s">
         <v>78</v>
       </c>
       <c r="C152" s="9"/>
       <c r="D152" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="29"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="27"/>
       <c r="C153" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D153" s="6"/>
     </row>
-    <row r="154" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="29"/>
+    <row r="154" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="27"/>
       <c r="C154" s="7"/>
       <c r="D154" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="156" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="157" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C157" s="25" t="s">
+      <c r="C157" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D157" s="27"/>
-    </row>
-    <row r="158" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D157" s="34"/>
+    </row>
+    <row r="158" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C158" s="25" t="s">
+      <c r="C158" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D158" s="27"/>
-    </row>
-    <row r="159" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D158" s="34"/>
+    </row>
+    <row r="159" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C159" s="25" t="s">
+      <c r="C159" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D159" s="27"/>
-    </row>
-    <row r="160" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D159" s="34"/>
+    </row>
+    <row r="160" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B160" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C160" s="25" t="s">
+      <c r="C160" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D160" s="27"/>
-    </row>
-    <row r="161" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D160" s="34"/>
+    </row>
+    <row r="161" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B161" s="28" t="s">
         <v>2</v>
       </c>
@@ -2356,47 +2347,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B162" s="28"/>
-      <c r="C162" s="34" t="s">
+      <c r="C162" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D162" s="35"/>
-    </row>
-    <row r="163" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D162" s="26"/>
+    </row>
+    <row r="163" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B163" s="28"/>
-      <c r="C163" s="34"/>
-      <c r="D163" s="35" t="s">
+      <c r="C163" s="25"/>
+      <c r="D163" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="164" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="28"/>
       <c r="C164" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D164" s="6"/>
     </row>
-    <row r="165" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B165" s="28"/>
       <c r="C165" s="5"/>
       <c r="D165" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="166" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="28"/>
       <c r="C166" s="5"/>
       <c r="D166" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="167" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B167" s="28"/>
       <c r="C167" s="7"/>
       <c r="D167" s="8"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="30" t="s">
         <v>103</v>
       </c>
@@ -2405,61 +2396,61 @@
         <v>101</v>
       </c>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B169" s="31"/>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="32"/>
       <c r="C169" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D169" s="6"/>
     </row>
-    <row r="170" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="32"/>
+    <row r="170" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="31"/>
       <c r="C170" s="7"/>
       <c r="D170" s="8"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="17"/>
       <c r="C171" s="24"/>
       <c r="D171" s="24"/>
     </row>
-    <row r="172" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="173" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="173" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B173" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C173" s="25" t="s">
+      <c r="C173" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D173" s="27"/>
-    </row>
-    <row r="174" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D173" s="34"/>
+    </row>
+    <row r="174" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B174" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C174" s="25" t="s">
+      <c r="C174" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D174" s="27"/>
-    </row>
-    <row r="175" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D174" s="34"/>
+    </row>
+    <row r="175" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B175" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C175" s="25" t="s">
+      <c r="C175" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D175" s="27"/>
-    </row>
-    <row r="176" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D175" s="34"/>
+    </row>
+    <row r="176" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C176" s="25" t="s">
+      <c r="C176" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D176" s="27"/>
-    </row>
-    <row r="177" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D176" s="34"/>
+    </row>
+    <row r="177" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="28" t="s">
         <v>2</v>
       </c>
@@ -2470,34 +2461,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B178" s="28"/>
       <c r="C178" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D178" s="6"/>
     </row>
-    <row r="179" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B179" s="28"/>
       <c r="C179" s="5"/>
       <c r="D179" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="180" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B180" s="28"/>
       <c r="C180" s="5"/>
       <c r="D180" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="181" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B181" s="28"/>
       <c r="C181" s="7"/>
       <c r="D181" s="8"/>
     </row>
-    <row r="182" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="29" t="s">
+    <row r="182" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="27" t="s">
         <v>83</v>
       </c>
       <c r="C182" s="9"/>
@@ -2505,49 +2496,49 @@
         <v>84</v>
       </c>
     </row>
-    <row r="183" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="29"/>
+    <row r="183" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="27"/>
       <c r="C183" s="7"/>
       <c r="D183" s="8"/>
     </row>
-    <row r="185" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B186" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C186" s="25" t="s">
+      <c r="C186" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D186" s="27"/>
-    </row>
-    <row r="187" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D186" s="34"/>
+    </row>
+    <row r="187" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B187" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C187" s="25" t="s">
+      <c r="C187" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D187" s="27"/>
-    </row>
-    <row r="188" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D187" s="34"/>
+    </row>
+    <row r="188" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B188" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C188" s="25" t="s">
+      <c r="C188" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="D188" s="27"/>
-    </row>
-    <row r="189" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D188" s="34"/>
+    </row>
+    <row r="189" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B189" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C189" s="25" t="s">
+      <c r="C189" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D189" s="27"/>
-    </row>
-    <row r="190" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D189" s="34"/>
+    </row>
+    <row r="190" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B190" s="28" t="s">
         <v>2</v>
       </c>
@@ -2558,34 +2549,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B191" s="28"/>
       <c r="C191" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D191" s="6"/>
     </row>
-    <row r="192" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B192" s="28"/>
       <c r="C192" s="5"/>
       <c r="D192" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="193" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B193" s="28"/>
       <c r="C193" s="5"/>
       <c r="D193" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B194" s="28"/>
       <c r="C194" s="7"/>
       <c r="D194" s="8"/>
     </row>
-    <row r="195" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="29" t="s">
+    <row r="195" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C195" s="9"/>
@@ -2593,61 +2584,61 @@
         <v>89</v>
       </c>
     </row>
-    <row r="196" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="29"/>
+    <row r="196" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="27"/>
       <c r="C196" s="5" t="s">
         <v>90</v>
       </c>
       <c r="D196" s="6"/>
     </row>
-    <row r="197" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="29"/>
+    <row r="197" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="27"/>
       <c r="C197" s="7"/>
       <c r="D197" s="8"/>
     </row>
-    <row r="198" spans="2:4" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:4" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="17"/>
       <c r="C198" s="18"/>
       <c r="D198" s="18"/>
     </row>
-    <row r="199" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="200" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B200" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C200" s="25" t="s">
+      <c r="C200" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D200" s="27"/>
-    </row>
-    <row r="201" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D200" s="34"/>
+    </row>
+    <row r="201" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C201" s="25" t="s">
+      <c r="C201" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D201" s="27"/>
-    </row>
-    <row r="202" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D201" s="34"/>
+    </row>
+    <row r="202" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C202" s="25" t="s">
+      <c r="C202" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D202" s="27"/>
-    </row>
-    <row r="203" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D202" s="34"/>
+    </row>
+    <row r="203" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B203" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C203" s="25" t="s">
+      <c r="C203" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D203" s="27"/>
-    </row>
-    <row r="204" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D203" s="34"/>
+    </row>
+    <row r="204" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B204" s="28" t="s">
         <v>2</v>
       </c>
@@ -2658,55 +2649,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B205" s="28"/>
       <c r="C205" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D205" s="6"/>
     </row>
-    <row r="206" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B206" s="28"/>
       <c r="C206" s="5"/>
       <c r="D206" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B207" s="28"/>
       <c r="C207" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D207" s="6"/>
     </row>
-    <row r="208" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B208" s="28"/>
       <c r="C208" s="5"/>
       <c r="D208" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="209" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B209" s="28"/>
       <c r="C209" s="5"/>
       <c r="D209" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B210" s="28"/>
       <c r="C210" s="5"/>
       <c r="D210" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B211" s="28"/>
       <c r="C211" s="7"/>
       <c r="D211" s="8"/>
     </row>
-    <row r="212" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="29" t="s">
+    <row r="212" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C212" s="9"/>
@@ -2714,58 +2705,58 @@
         <v>104</v>
       </c>
     </row>
-    <row r="213" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B213" s="29"/>
+    <row r="213" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B213" s="27"/>
       <c r="C213" s="5" t="s">
         <v>105</v>
       </c>
       <c r="D213" s="6"/>
     </row>
-    <row r="214" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B214" s="29"/>
+    <row r="214" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B214" s="27"/>
       <c r="C214" s="7"/>
       <c r="D214" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="216" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="217" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B217" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C217" s="25" t="s">
+      <c r="C217" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D217" s="27"/>
-    </row>
-    <row r="218" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D217" s="34"/>
+    </row>
+    <row r="218" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B218" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C218" s="25" t="s">
+      <c r="C218" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D218" s="27"/>
-    </row>
-    <row r="219" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D218" s="34"/>
+    </row>
+    <row r="219" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B219" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C219" s="25" t="s">
+      <c r="C219" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D219" s="27"/>
-    </row>
-    <row r="220" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D219" s="34"/>
+    </row>
+    <row r="220" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B220" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C220" s="25" t="s">
+      <c r="C220" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D220" s="27"/>
-    </row>
-    <row r="221" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D220" s="34"/>
+    </row>
+    <row r="221" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B221" s="28" t="s">
         <v>2</v>
       </c>
@@ -2776,28 +2767,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B222" s="28"/>
-      <c r="C222" s="34" t="s">
+      <c r="C222" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D222" s="35"/>
-    </row>
-    <row r="223" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D222" s="26"/>
+    </row>
+    <row r="223" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B223" s="28"/>
-      <c r="C223" s="34"/>
-      <c r="D223" s="35" t="s">
+      <c r="C223" s="25"/>
+      <c r="D223" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="224" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B224" s="28"/>
-      <c r="C224" s="34" t="s">
+      <c r="C224" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D224" s="35"/>
-    </row>
-    <row r="225" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D224" s="26"/>
+    </row>
+    <row r="225" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B225" s="28"/>
       <c r="C225" s="5" t="s">
         <v>94</v>
@@ -2805,28 +2796,82 @@
       <c r="D225" s="6"/>
       <c r="N225" s="13"/>
     </row>
-    <row r="226" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B226" s="28"/>
       <c r="C226" s="5"/>
       <c r="D226" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="227" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B227" s="28"/>
       <c r="C227" s="7"/>
       <c r="D227" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C219:D219"/>
+    <mergeCell ref="C188:D188"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C186:D186"/>
+    <mergeCell ref="C187:D187"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C200:D200"/>
+    <mergeCell ref="C201:D201"/>
+    <mergeCell ref="C189:D189"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="B221:B227"/>
+    <mergeCell ref="B177:B181"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C175:D175"/>
+    <mergeCell ref="C176:D176"/>
+    <mergeCell ref="C220:D220"/>
+    <mergeCell ref="C202:D202"/>
+    <mergeCell ref="C217:D217"/>
+    <mergeCell ref="C218:D218"/>
+    <mergeCell ref="B168:B170"/>
+    <mergeCell ref="B190:B194"/>
+    <mergeCell ref="B195:B197"/>
+    <mergeCell ref="B204:B211"/>
+    <mergeCell ref="B212:B214"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B59:B61"/>
@@ -2843,69 +2888,15 @@
     <mergeCell ref="B105:B107"/>
     <mergeCell ref="C123:D123"/>
     <mergeCell ref="C111:D111"/>
-    <mergeCell ref="B168:B170"/>
-    <mergeCell ref="B190:B194"/>
-    <mergeCell ref="B195:B197"/>
-    <mergeCell ref="B204:B211"/>
-    <mergeCell ref="B212:B214"/>
-    <mergeCell ref="B221:B227"/>
-    <mergeCell ref="B177:B181"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C159:D159"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C175:D175"/>
-    <mergeCell ref="C176:D176"/>
-    <mergeCell ref="C220:D220"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B41:B43"/>
     <mergeCell ref="B71:B76"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C200:D200"/>
-    <mergeCell ref="C201:D201"/>
-    <mergeCell ref="C202:D202"/>
-    <mergeCell ref="C217:D217"/>
-    <mergeCell ref="C218:D218"/>
-    <mergeCell ref="C189:D189"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C219:D219"/>
-    <mergeCell ref="C188:D188"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C186:D186"/>
-    <mergeCell ref="C187:D187"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>